<commit_message>
Update of knowledge base Rename of mockup knowledge base
</commit_message>
<xml_diff>
--- a/resources/KnowledgeBase.xlsx
+++ b/resources/KnowledgeBase.xlsx
@@ -1303,30 +1303,6 @@
     <author>Metz</author>
   </authors>
   <commentList>
-    <comment ref="Q12" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Metz:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Might be Influencing in case Free Pricing model because private cloud is unlikely to be free.</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="N18" authorId="0" shapeId="0">
       <text>
         <r>
@@ -2878,11 +2854,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2911,10 +2887,16 @@
     <xf numFmtId="49" fontId="10" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="10" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2926,28 +2908,19 @@
     <xf numFmtId="49" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="10" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2977,11 +2950,14 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -3790,9 +3766,9 @@
     <col min="1" max="1" width="16.7109375" style="106" customWidth="1"/>
     <col min="2" max="2" width="15.42578125" style="94" customWidth="1"/>
     <col min="3" max="3" width="48.85546875" style="99" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.140625" style="95" customWidth="1"/>
-    <col min="5" max="5" width="23.7109375" style="102" customWidth="1"/>
-    <col min="6" max="6" width="50.5703125" style="97" customWidth="1"/>
+    <col min="4" max="4" width="32.140625" style="95" customWidth="1"/>
+    <col min="5" max="5" width="26.85546875" style="102" customWidth="1"/>
+    <col min="6" max="6" width="55.140625" style="97" customWidth="1"/>
     <col min="7" max="7" width="28" style="102" customWidth="1"/>
     <col min="8" max="8" width="26.28515625" style="102" customWidth="1"/>
     <col min="9" max="9" width="42.28515625" style="96" customWidth="1"/>
@@ -3837,10 +3813,10 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="129" t="s">
+      <c r="A2" s="130" t="s">
         <v>170</v>
       </c>
-      <c r="B2" s="129" t="s">
+      <c r="B2" s="130" t="s">
         <v>55</v>
       </c>
       <c r="C2" s="99" t="s">
@@ -3863,8 +3839,8 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="129"/>
-      <c r="B3" s="129"/>
+      <c r="A3" s="130"/>
+      <c r="B3" s="130"/>
       <c r="C3" s="99" t="s">
         <v>5</v>
       </c>
@@ -3877,8 +3853,8 @@
       <c r="H3" s="128"/>
     </row>
     <row r="4" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="129"/>
-      <c r="B4" s="129"/>
+      <c r="A4" s="130"/>
+      <c r="B4" s="130"/>
       <c r="C4" s="99" t="s">
         <v>48</v>
       </c>
@@ -3891,8 +3867,8 @@
       <c r="H4" s="128"/>
     </row>
     <row r="5" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="129"/>
-      <c r="B5" s="129"/>
+      <c r="A5" s="130"/>
+      <c r="B5" s="130"/>
       <c r="C5" s="99" t="s">
         <v>46</v>
       </c>
@@ -3905,8 +3881,8 @@
       <c r="H5" s="128"/>
     </row>
     <row r="6" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="129"/>
-      <c r="B6" s="129"/>
+      <c r="A6" s="130"/>
+      <c r="B6" s="130"/>
       <c r="C6" s="99" t="s">
         <v>49</v>
       </c>
@@ -3919,8 +3895,8 @@
       <c r="H6" s="128"/>
     </row>
     <row r="7" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="129"/>
-      <c r="B7" s="129"/>
+      <c r="A7" s="130"/>
+      <c r="B7" s="130"/>
       <c r="C7" s="99" t="s">
         <v>50</v>
       </c>
@@ -3933,8 +3909,8 @@
       <c r="H7" s="128"/>
     </row>
     <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="129"/>
-      <c r="B8" s="129"/>
+      <c r="A8" s="130"/>
+      <c r="B8" s="130"/>
       <c r="C8" s="99" t="s">
         <v>51</v>
       </c>
@@ -3947,8 +3923,8 @@
       <c r="H8" s="128"/>
     </row>
     <row r="9" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="129"/>
-      <c r="B9" s="129" t="s">
+      <c r="A9" s="130"/>
+      <c r="B9" s="130" t="s">
         <v>56</v>
       </c>
       <c r="C9" s="99" t="s">
@@ -3967,8 +3943,8 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="129"/>
-      <c r="B10" s="129"/>
+      <c r="A10" s="130"/>
+      <c r="B10" s="130"/>
       <c r="C10" s="99" t="s">
         <v>2</v>
       </c>
@@ -3981,8 +3957,8 @@
       <c r="H10" s="128"/>
     </row>
     <row r="11" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="129"/>
-      <c r="B11" s="129"/>
+      <c r="A11" s="130"/>
+      <c r="B11" s="130"/>
       <c r="C11" s="99" t="s">
         <v>6</v>
       </c>
@@ -3995,8 +3971,8 @@
       <c r="H11" s="128"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="129"/>
-      <c r="B12" s="129"/>
+      <c r="A12" s="130"/>
+      <c r="B12" s="130"/>
       <c r="C12" s="99" t="s">
         <v>52</v>
       </c>
@@ -4009,8 +3985,8 @@
       <c r="H12" s="128"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="129"/>
-      <c r="B13" s="129"/>
+      <c r="A13" s="130"/>
+      <c r="B13" s="130"/>
       <c r="C13" s="99" t="s">
         <v>53</v>
       </c>
@@ -4023,8 +3999,8 @@
       <c r="H13" s="128"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="129"/>
-      <c r="B14" s="129"/>
+      <c r="A14" s="130"/>
+      <c r="B14" s="130"/>
       <c r="C14" s="99" t="s">
         <v>37</v>
       </c>
@@ -4037,8 +4013,8 @@
       <c r="H14" s="128"/>
     </row>
     <row r="15" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="129"/>
-      <c r="B15" s="129"/>
+      <c r="A15" s="130"/>
+      <c r="B15" s="130"/>
       <c r="C15" s="99" t="s">
         <v>54</v>
       </c>
@@ -4051,8 +4027,8 @@
       <c r="H15" s="128"/>
     </row>
     <row r="16" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="129"/>
-      <c r="B16" s="129" t="s">
+      <c r="A16" s="130"/>
+      <c r="B16" s="130" t="s">
         <v>57</v>
       </c>
       <c r="C16" s="99" t="s">
@@ -4071,8 +4047,8 @@
       </c>
     </row>
     <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="129"/>
-      <c r="B17" s="129"/>
+      <c r="A17" s="130"/>
+      <c r="B17" s="130"/>
       <c r="C17" s="99" t="s">
         <v>3</v>
       </c>
@@ -4085,8 +4061,8 @@
       <c r="H17" s="128"/>
     </row>
     <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="129"/>
-      <c r="B18" s="129"/>
+      <c r="A18" s="130"/>
+      <c r="B18" s="130"/>
       <c r="C18" s="99" t="s">
         <v>30</v>
       </c>
@@ -4099,8 +4075,8 @@
       <c r="H18" s="128"/>
     </row>
     <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="129"/>
-      <c r="B19" s="129"/>
+      <c r="A19" s="130"/>
+      <c r="B19" s="130"/>
       <c r="C19" s="99" t="s">
         <v>38</v>
       </c>
@@ -4113,8 +4089,8 @@
       <c r="H19" s="128"/>
     </row>
     <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="129"/>
-      <c r="B20" s="129"/>
+      <c r="A20" s="130"/>
+      <c r="B20" s="130"/>
       <c r="C20" s="99" t="s">
         <v>63</v>
       </c>
@@ -4127,8 +4103,8 @@
       <c r="H20" s="128"/>
     </row>
     <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="129"/>
-      <c r="B21" s="129"/>
+      <c r="A21" s="130"/>
+      <c r="B21" s="130"/>
       <c r="C21" s="99" t="s">
         <v>62</v>
       </c>
@@ -4141,8 +4117,8 @@
       <c r="H21" s="128"/>
     </row>
     <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="129"/>
-      <c r="B22" s="129"/>
+      <c r="A22" s="130"/>
+      <c r="B22" s="130"/>
       <c r="C22" s="99" t="s">
         <v>64</v>
       </c>
@@ -4155,8 +4131,8 @@
       <c r="H22" s="128"/>
     </row>
     <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="129"/>
-      <c r="B23" s="129"/>
+      <c r="A23" s="130"/>
+      <c r="B23" s="130"/>
       <c r="C23" s="99" t="s">
         <v>31</v>
       </c>
@@ -4169,8 +4145,8 @@
       <c r="H23" s="128"/>
     </row>
     <row r="24" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="129"/>
-      <c r="B24" s="129" t="s">
+      <c r="A24" s="130"/>
+      <c r="B24" s="130" t="s">
         <v>69</v>
       </c>
       <c r="C24" s="99" t="s">
@@ -4189,8 +4165,8 @@
       </c>
     </row>
     <row r="25" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="129"/>
-      <c r="B25" s="129"/>
+      <c r="A25" s="130"/>
+      <c r="B25" s="130"/>
       <c r="C25" s="99" t="s">
         <v>59</v>
       </c>
@@ -4203,8 +4179,8 @@
       <c r="H25" s="128"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="129"/>
-      <c r="B26" s="129"/>
+      <c r="A26" s="130"/>
+      <c r="B26" s="130"/>
       <c r="C26" s="99" t="s">
         <v>60</v>
       </c>
@@ -4217,8 +4193,8 @@
       <c r="H26" s="128"/>
     </row>
     <row r="27" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="129"/>
-      <c r="B27" s="129"/>
+      <c r="A27" s="130"/>
+      <c r="B27" s="130"/>
       <c r="C27" s="99" t="s">
         <v>61</v>
       </c>
@@ -4231,10 +4207,10 @@
       <c r="H27" s="128"/>
     </row>
     <row r="28" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="129" t="s">
+      <c r="A28" s="130" t="s">
         <v>7</v>
       </c>
-      <c r="B28" s="129" t="s">
+      <c r="B28" s="130" t="s">
         <v>70</v>
       </c>
       <c r="C28" s="103" t="s">
@@ -4249,16 +4225,16 @@
       <c r="F28" s="98" t="s">
         <v>224</v>
       </c>
-      <c r="G28" s="130" t="s">
+      <c r="G28" s="129" t="s">
         <v>91</v>
       </c>
-      <c r="H28" s="130" t="s">
+      <c r="H28" s="129" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A29" s="129"/>
-      <c r="B29" s="129"/>
+      <c r="A29" s="130"/>
+      <c r="B29" s="130"/>
       <c r="C29" s="99" t="s">
         <v>176</v>
       </c>
@@ -4267,12 +4243,12 @@
       <c r="F29" s="98" t="s">
         <v>125</v>
       </c>
-      <c r="G29" s="130"/>
-      <c r="H29" s="130"/>
+      <c r="G29" s="129"/>
+      <c r="H29" s="129"/>
     </row>
     <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="129"/>
-      <c r="B30" s="129"/>
+      <c r="A30" s="130"/>
+      <c r="B30" s="130"/>
       <c r="C30" s="99" t="s">
         <v>23</v>
       </c>
@@ -4281,12 +4257,12 @@
       <c r="F30" s="98" t="s">
         <v>130</v>
       </c>
-      <c r="G30" s="130"/>
-      <c r="H30" s="130"/>
+      <c r="G30" s="129"/>
+      <c r="H30" s="129"/>
     </row>
     <row r="31" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A31" s="129"/>
-      <c r="B31" s="129"/>
+      <c r="A31" s="130"/>
+      <c r="B31" s="130"/>
       <c r="C31" s="99" t="s">
         <v>22</v>
       </c>
@@ -4295,12 +4271,12 @@
       <c r="F31" s="98" t="s">
         <v>126</v>
       </c>
-      <c r="G31" s="130"/>
-      <c r="H31" s="130"/>
+      <c r="G31" s="129"/>
+      <c r="H31" s="129"/>
     </row>
     <row r="32" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="129"/>
-      <c r="B32" s="129"/>
+      <c r="A32" s="130"/>
+      <c r="B32" s="130"/>
       <c r="C32" s="99" t="s">
         <v>175</v>
       </c>
@@ -4309,12 +4285,12 @@
       <c r="F32" s="97" t="s">
         <v>196</v>
       </c>
-      <c r="G32" s="130"/>
-      <c r="H32" s="130"/>
+      <c r="G32" s="129"/>
+      <c r="H32" s="129"/>
     </row>
     <row r="33" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="129"/>
-      <c r="B33" s="129"/>
+      <c r="A33" s="130"/>
+      <c r="B33" s="130"/>
       <c r="C33" s="99" t="s">
         <v>177</v>
       </c>
@@ -4323,12 +4299,12 @@
       <c r="F33" s="97" t="s">
         <v>131</v>
       </c>
-      <c r="G33" s="130"/>
-      <c r="H33" s="130"/>
+      <c r="G33" s="129"/>
+      <c r="H33" s="129"/>
     </row>
     <row r="34" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="129"/>
-      <c r="B34" s="129"/>
+      <c r="A34" s="130"/>
+      <c r="B34" s="130"/>
       <c r="C34" s="99" t="s">
         <v>81</v>
       </c>
@@ -4337,12 +4313,12 @@
       <c r="F34" s="97" t="s">
         <v>127</v>
       </c>
-      <c r="G34" s="130"/>
-      <c r="H34" s="130"/>
+      <c r="G34" s="129"/>
+      <c r="H34" s="129"/>
     </row>
     <row r="35" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="129"/>
-      <c r="B35" s="129"/>
+      <c r="A35" s="130"/>
+      <c r="B35" s="130"/>
       <c r="C35" s="99" t="s">
         <v>178</v>
       </c>
@@ -4351,12 +4327,12 @@
       <c r="F35" s="97" t="s">
         <v>132</v>
       </c>
-      <c r="G35" s="130"/>
-      <c r="H35" s="130"/>
+      <c r="G35" s="129"/>
+      <c r="H35" s="129"/>
     </row>
     <row r="36" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A36" s="129"/>
-      <c r="B36" s="129" t="s">
+      <c r="A36" s="130"/>
+      <c r="B36" s="130" t="s">
         <v>71</v>
       </c>
       <c r="C36" s="99" t="s">
@@ -4369,14 +4345,14 @@
       <c r="F36" s="97" t="s">
         <v>133</v>
       </c>
-      <c r="G36" s="130"/>
+      <c r="G36" s="129"/>
       <c r="H36" s="128" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="129"/>
-      <c r="B37" s="129"/>
+      <c r="A37" s="130"/>
+      <c r="B37" s="130"/>
       <c r="C37" s="99" t="s">
         <v>24</v>
       </c>
@@ -4385,12 +4361,12 @@
       <c r="F37" s="97" t="s">
         <v>225</v>
       </c>
-      <c r="G37" s="130"/>
+      <c r="G37" s="129"/>
       <c r="H37" s="128"/>
     </row>
     <row r="38" spans="1:9" s="99" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="129"/>
-      <c r="B38" s="129"/>
+      <c r="A38" s="130"/>
+      <c r="B38" s="130"/>
       <c r="C38" s="99" t="s">
         <v>9</v>
       </c>
@@ -4399,12 +4375,12 @@
       <c r="F38" s="100" t="s">
         <v>134</v>
       </c>
-      <c r="G38" s="130"/>
+      <c r="G38" s="129"/>
       <c r="H38" s="128"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="129"/>
-      <c r="B39" s="129" t="s">
+      <c r="A39" s="130"/>
+      <c r="B39" s="130" t="s">
         <v>72</v>
       </c>
       <c r="C39" s="99" t="s">
@@ -4417,14 +4393,14 @@
       <c r="F39" s="97" t="s">
         <v>135</v>
       </c>
-      <c r="G39" s="130"/>
+      <c r="G39" s="129"/>
       <c r="H39" s="128" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A40" s="129"/>
-      <c r="B40" s="129"/>
+      <c r="A40" s="130"/>
+      <c r="B40" s="130"/>
       <c r="C40" s="99" t="s">
         <v>11</v>
       </c>
@@ -4433,12 +4409,12 @@
       <c r="F40" s="97" t="s">
         <v>226</v>
       </c>
-      <c r="G40" s="130"/>
+      <c r="G40" s="129"/>
       <c r="H40" s="128"/>
     </row>
     <row r="41" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A41" s="129"/>
-      <c r="B41" s="129"/>
+      <c r="A41" s="130"/>
+      <c r="B41" s="130"/>
       <c r="C41" s="99" t="s">
         <v>65</v>
       </c>
@@ -4447,12 +4423,12 @@
       <c r="F41" s="97" t="s">
         <v>227</v>
       </c>
-      <c r="G41" s="130"/>
+      <c r="G41" s="129"/>
       <c r="H41" s="128"/>
     </row>
     <row r="42" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="129"/>
-      <c r="B42" s="129"/>
+      <c r="A42" s="130"/>
+      <c r="B42" s="130"/>
       <c r="C42" s="99" t="s">
         <v>12</v>
       </c>
@@ -4461,12 +4437,12 @@
       <c r="F42" s="97" t="s">
         <v>136</v>
       </c>
-      <c r="G42" s="130"/>
+      <c r="G42" s="129"/>
       <c r="H42" s="128"/>
     </row>
     <row r="43" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A43" s="129"/>
-      <c r="B43" s="129"/>
+      <c r="A43" s="130"/>
+      <c r="B43" s="130"/>
       <c r="C43" s="99" t="s">
         <v>66</v>
       </c>
@@ -4475,12 +4451,12 @@
       <c r="F43" s="97" t="s">
         <v>228</v>
       </c>
-      <c r="G43" s="130"/>
+      <c r="G43" s="129"/>
       <c r="H43" s="128"/>
     </row>
     <row r="44" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" s="129"/>
-      <c r="B44" s="129" t="s">
+      <c r="A44" s="130"/>
+      <c r="B44" s="130" t="s">
         <v>73</v>
       </c>
       <c r="C44" s="99" t="s">
@@ -4493,14 +4469,14 @@
       <c r="F44" s="97" t="s">
         <v>137</v>
       </c>
-      <c r="G44" s="130"/>
+      <c r="G44" s="129"/>
       <c r="H44" s="128" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="129"/>
-      <c r="B45" s="129"/>
+      <c r="A45" s="130"/>
+      <c r="B45" s="130"/>
       <c r="C45" s="99" t="s">
         <v>26</v>
       </c>
@@ -4509,12 +4485,12 @@
       <c r="F45" s="97" t="s">
         <v>138</v>
       </c>
-      <c r="G45" s="130"/>
+      <c r="G45" s="129"/>
       <c r="H45" s="128"/>
     </row>
     <row r="46" spans="1:9" s="99" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A46" s="129"/>
-      <c r="B46" s="129"/>
+      <c r="A46" s="130"/>
+      <c r="B46" s="130"/>
       <c r="C46" s="99" t="s">
         <v>27</v>
       </c>
@@ -4523,14 +4499,14 @@
       <c r="F46" s="100" t="s">
         <v>197</v>
       </c>
-      <c r="G46" s="130"/>
+      <c r="G46" s="129"/>
       <c r="H46" s="128"/>
     </row>
     <row r="47" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A47" s="129" t="s">
+      <c r="A47" s="130" t="s">
         <v>82</v>
       </c>
-      <c r="B47" s="129" t="s">
+      <c r="B47" s="130" t="s">
         <v>181</v>
       </c>
       <c r="C47" s="99" t="s">
@@ -4554,8 +4530,8 @@
       <c r="I47" s="110"/>
     </row>
     <row r="48" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A48" s="129"/>
-      <c r="B48" s="129"/>
+      <c r="A48" s="130"/>
+      <c r="B48" s="130"/>
       <c r="C48" s="99" t="s">
         <v>172</v>
       </c>
@@ -4569,8 +4545,8 @@
       <c r="I48" s="110"/>
     </row>
     <row r="49" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A49" s="129"/>
-      <c r="B49" s="129"/>
+      <c r="A49" s="130"/>
+      <c r="B49" s="130"/>
       <c r="C49" s="99" t="s">
         <v>173</v>
       </c>
@@ -4584,8 +4560,8 @@
       <c r="I49" s="110"/>
     </row>
     <row r="50" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A50" s="129"/>
-      <c r="B50" s="129"/>
+      <c r="A50" s="130"/>
+      <c r="B50" s="130"/>
       <c r="C50" s="99" t="s">
         <v>174</v>
       </c>
@@ -4599,10 +4575,10 @@
       <c r="I50" s="110"/>
     </row>
     <row r="51" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A51" s="129" t="s">
+      <c r="A51" s="130" t="s">
         <v>83</v>
       </c>
-      <c r="B51" s="129" t="s">
+      <c r="B51" s="130" t="s">
         <v>74</v>
       </c>
       <c r="C51" s="99" t="s">
@@ -4625,8 +4601,8 @@
       </c>
     </row>
     <row r="52" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A52" s="129"/>
-      <c r="B52" s="129"/>
+      <c r="A52" s="130"/>
+      <c r="B52" s="130"/>
       <c r="C52" s="99" t="s">
         <v>13</v>
       </c>
@@ -4639,8 +4615,8 @@
       <c r="H52" s="128"/>
     </row>
     <row r="53" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A53" s="129"/>
-      <c r="B53" s="129"/>
+      <c r="A53" s="130"/>
+      <c r="B53" s="130"/>
       <c r="C53" s="99" t="s">
         <v>14</v>
       </c>
@@ -4653,8 +4629,8 @@
       <c r="H53" s="128"/>
     </row>
     <row r="54" spans="1:9" s="99" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A54" s="129"/>
-      <c r="B54" s="129"/>
+      <c r="A54" s="130"/>
+      <c r="B54" s="130"/>
       <c r="C54" s="99" t="s">
         <v>67</v>
       </c>
@@ -4667,8 +4643,8 @@
       <c r="H54" s="128"/>
     </row>
     <row r="55" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A55" s="129"/>
-      <c r="B55" s="129" t="s">
+      <c r="A55" s="130"/>
+      <c r="B55" s="130" t="s">
         <v>75</v>
       </c>
       <c r="C55" s="99" t="s">
@@ -4687,8 +4663,8 @@
       </c>
     </row>
     <row r="56" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A56" s="129"/>
-      <c r="B56" s="129"/>
+      <c r="A56" s="130"/>
+      <c r="B56" s="130"/>
       <c r="C56" s="99" t="s">
         <v>28</v>
       </c>
@@ -4701,8 +4677,8 @@
       <c r="H56" s="128"/>
     </row>
     <row r="57" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A57" s="129"/>
-      <c r="B57" s="129"/>
+      <c r="A57" s="130"/>
+      <c r="B57" s="130"/>
       <c r="C57" s="99" t="s">
         <v>16</v>
       </c>
@@ -4715,8 +4691,8 @@
       <c r="H57" s="128"/>
     </row>
     <row r="58" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A58" s="129"/>
-      <c r="B58" s="129"/>
+      <c r="A58" s="130"/>
+      <c r="B58" s="130"/>
       <c r="C58" s="99" t="s">
         <v>43</v>
       </c>
@@ -4729,8 +4705,8 @@
       <c r="H58" s="128"/>
     </row>
     <row r="59" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A59" s="129"/>
-      <c r="B59" s="129"/>
+      <c r="A59" s="130"/>
+      <c r="B59" s="130"/>
       <c r="C59" s="99" t="s">
         <v>44</v>
       </c>
@@ -4743,8 +4719,8 @@
       <c r="H59" s="128"/>
     </row>
     <row r="60" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A60" s="129"/>
-      <c r="B60" s="129"/>
+      <c r="A60" s="130"/>
+      <c r="B60" s="130"/>
       <c r="C60" s="99" t="s">
         <v>45</v>
       </c>
@@ -4757,8 +4733,8 @@
       <c r="H60" s="128"/>
     </row>
     <row r="61" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A61" s="129"/>
-      <c r="B61" s="129"/>
+      <c r="A61" s="130"/>
+      <c r="B61" s="130"/>
       <c r="C61" s="99" t="s">
         <v>68</v>
       </c>
@@ -4771,8 +4747,8 @@
       <c r="H61" s="128"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A62" s="129"/>
-      <c r="B62" s="129" t="s">
+      <c r="A62" s="130"/>
+      <c r="B62" s="130" t="s">
         <v>76</v>
       </c>
       <c r="C62" s="99" t="s">
@@ -4791,8 +4767,8 @@
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A63" s="129"/>
-      <c r="B63" s="129"/>
+      <c r="A63" s="130"/>
+      <c r="B63" s="130"/>
       <c r="C63" s="99" t="s">
         <v>40</v>
       </c>
@@ -4805,8 +4781,8 @@
       <c r="H63" s="128"/>
     </row>
     <row r="64" spans="1:9" s="99" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A64" s="129"/>
-      <c r="B64" s="129"/>
+      <c r="A64" s="130"/>
+      <c r="B64" s="130"/>
       <c r="C64" s="99" t="s">
         <v>18</v>
       </c>
@@ -4819,8 +4795,8 @@
       <c r="H64" s="128"/>
     </row>
     <row r="65" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A65" s="129"/>
-      <c r="B65" s="129" t="s">
+      <c r="A65" s="130"/>
+      <c r="B65" s="130" t="s">
         <v>77</v>
       </c>
       <c r="C65" s="99" t="s">
@@ -4839,8 +4815,8 @@
       </c>
     </row>
     <row r="66" spans="1:8" s="101" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A66" s="129"/>
-      <c r="B66" s="129"/>
+      <c r="A66" s="130"/>
+      <c r="B66" s="130"/>
       <c r="C66" s="99" t="s">
         <v>205</v>
       </c>
@@ -4853,8 +4829,8 @@
       <c r="H66" s="128"/>
     </row>
     <row r="67" spans="1:8" s="101" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A67" s="129"/>
-      <c r="B67" s="129"/>
+      <c r="A67" s="130"/>
+      <c r="B67" s="130"/>
       <c r="C67" s="99" t="s">
         <v>206</v>
       </c>
@@ -4867,8 +4843,8 @@
       <c r="H67" s="128"/>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A68" s="129"/>
-      <c r="B68" s="129"/>
+      <c r="A68" s="130"/>
+      <c r="B68" s="130"/>
       <c r="C68" s="99" t="s">
         <v>207</v>
       </c>
@@ -4881,8 +4857,8 @@
       <c r="H68" s="128"/>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A69" s="129"/>
-      <c r="B69" s="129"/>
+      <c r="A69" s="130"/>
+      <c r="B69" s="130"/>
       <c r="C69" s="99" t="s">
         <v>208</v>
       </c>
@@ -4895,8 +4871,8 @@
       <c r="H69" s="128"/>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A70" s="129"/>
-      <c r="B70" s="129"/>
+      <c r="A70" s="130"/>
+      <c r="B70" s="130"/>
       <c r="C70" s="99" t="s">
         <v>209</v>
       </c>
@@ -4909,8 +4885,8 @@
       <c r="H70" s="128"/>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A71" s="129"/>
-      <c r="B71" s="129"/>
+      <c r="A71" s="130"/>
+      <c r="B71" s="130"/>
       <c r="C71" s="99" t="s">
         <v>210</v>
       </c>
@@ -4923,7 +4899,7 @@
       <c r="H71" s="128"/>
     </row>
     <row r="72" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A72" s="129"/>
+      <c r="A72" s="130"/>
       <c r="B72" s="94" t="s">
         <v>78</v>
       </c>
@@ -4943,8 +4919,8 @@
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A73" s="129"/>
-      <c r="B73" s="129" t="s">
+      <c r="A73" s="130"/>
+      <c r="B73" s="130" t="s">
         <v>80</v>
       </c>
       <c r="C73" s="99" t="s">
@@ -4963,8 +4939,8 @@
       </c>
     </row>
     <row r="74" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A74" s="129"/>
-      <c r="B74" s="129"/>
+      <c r="A74" s="130"/>
+      <c r="B74" s="130"/>
       <c r="C74" s="99" t="s">
         <v>34</v>
       </c>
@@ -4977,8 +4953,8 @@
       <c r="H74" s="128"/>
     </row>
     <row r="75" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A75" s="129"/>
-      <c r="B75" s="129"/>
+      <c r="A75" s="130"/>
+      <c r="B75" s="130"/>
       <c r="C75" s="99" t="s">
         <v>35</v>
       </c>
@@ -4991,8 +4967,8 @@
       <c r="H75" s="128"/>
     </row>
     <row r="76" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A76" s="129"/>
-      <c r="B76" s="129"/>
+      <c r="A76" s="130"/>
+      <c r="B76" s="130"/>
       <c r="C76" s="99" t="s">
         <v>36</v>
       </c>
@@ -5005,8 +4981,8 @@
       <c r="H76" s="128"/>
     </row>
     <row r="77" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A77" s="129"/>
-      <c r="B77" s="129" t="s">
+      <c r="A77" s="130"/>
+      <c r="B77" s="130" t="s">
         <v>79</v>
       </c>
       <c r="C77" s="99" t="s">
@@ -5025,8 +5001,8 @@
       </c>
     </row>
     <row r="78" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A78" s="129"/>
-      <c r="B78" s="129"/>
+      <c r="A78" s="130"/>
+      <c r="B78" s="130"/>
       <c r="C78" s="107" t="s">
         <v>180</v>
       </c>
@@ -5041,6 +5017,47 @@
   </sheetData>
   <autoFilter ref="B1:I78"/>
   <mergeCells count="57">
+    <mergeCell ref="E51:E54"/>
+    <mergeCell ref="B51:B54"/>
+    <mergeCell ref="B55:B61"/>
+    <mergeCell ref="B47:B50"/>
+    <mergeCell ref="D28:D46"/>
+    <mergeCell ref="D47:D50"/>
+    <mergeCell ref="D51:D78"/>
+    <mergeCell ref="E77:E78"/>
+    <mergeCell ref="E28:E35"/>
+    <mergeCell ref="E36:E38"/>
+    <mergeCell ref="E39:E43"/>
+    <mergeCell ref="E44:E46"/>
+    <mergeCell ref="E47:E50"/>
+    <mergeCell ref="E55:E61"/>
+    <mergeCell ref="E62:E64"/>
+    <mergeCell ref="E65:E71"/>
+    <mergeCell ref="A2:A27"/>
+    <mergeCell ref="A28:A46"/>
+    <mergeCell ref="A47:A50"/>
+    <mergeCell ref="A51:A78"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="B2:B8"/>
+    <mergeCell ref="B16:B23"/>
+    <mergeCell ref="B24:B27"/>
+    <mergeCell ref="B28:B35"/>
+    <mergeCell ref="B9:B15"/>
+    <mergeCell ref="B65:B71"/>
+    <mergeCell ref="B73:B76"/>
+    <mergeCell ref="B77:B78"/>
+    <mergeCell ref="B62:B64"/>
+    <mergeCell ref="B39:B43"/>
+    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="H36:H38"/>
+    <mergeCell ref="H39:H43"/>
+    <mergeCell ref="H44:H46"/>
+    <mergeCell ref="G47:G50"/>
+    <mergeCell ref="D2:D27"/>
+    <mergeCell ref="E2:E8"/>
+    <mergeCell ref="E9:E15"/>
+    <mergeCell ref="E16:E23"/>
+    <mergeCell ref="E24:E27"/>
     <mergeCell ref="E73:E76"/>
     <mergeCell ref="G2:G27"/>
     <mergeCell ref="H77:H78"/>
@@ -5057,47 +5074,6 @@
     <mergeCell ref="G51:G78"/>
     <mergeCell ref="H28:H35"/>
     <mergeCell ref="G28:G46"/>
-    <mergeCell ref="H36:H38"/>
-    <mergeCell ref="H39:H43"/>
-    <mergeCell ref="H44:H46"/>
-    <mergeCell ref="G47:G50"/>
-    <mergeCell ref="D2:D27"/>
-    <mergeCell ref="E2:E8"/>
-    <mergeCell ref="E9:E15"/>
-    <mergeCell ref="E16:E23"/>
-    <mergeCell ref="E24:E27"/>
-    <mergeCell ref="A2:A27"/>
-    <mergeCell ref="A28:A46"/>
-    <mergeCell ref="A47:A50"/>
-    <mergeCell ref="A51:A78"/>
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="B2:B8"/>
-    <mergeCell ref="B16:B23"/>
-    <mergeCell ref="B24:B27"/>
-    <mergeCell ref="B28:B35"/>
-    <mergeCell ref="B9:B15"/>
-    <mergeCell ref="B65:B71"/>
-    <mergeCell ref="B73:B76"/>
-    <mergeCell ref="B77:B78"/>
-    <mergeCell ref="B62:B64"/>
-    <mergeCell ref="B39:B43"/>
-    <mergeCell ref="B44:B46"/>
-    <mergeCell ref="E51:E54"/>
-    <mergeCell ref="B51:B54"/>
-    <mergeCell ref="B55:B61"/>
-    <mergeCell ref="B47:B50"/>
-    <mergeCell ref="D28:D46"/>
-    <mergeCell ref="D47:D50"/>
-    <mergeCell ref="D51:D78"/>
-    <mergeCell ref="E77:E78"/>
-    <mergeCell ref="E28:E35"/>
-    <mergeCell ref="E36:E38"/>
-    <mergeCell ref="E39:E43"/>
-    <mergeCell ref="E44:E46"/>
-    <mergeCell ref="E47:E50"/>
-    <mergeCell ref="E55:E61"/>
-    <mergeCell ref="E62:E64"/>
-    <mergeCell ref="E65:E71"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5117,7 +5093,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="O14" sqref="O14"/>
+      <selection pane="bottomRight" activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7737,145 +7713,145 @@
         <v>1</v>
       </c>
       <c r="B2" s="117"/>
-      <c r="D2" s="151" t="str">
+      <c r="D2" s="148" t="str">
         <f>'Knowledge Base'!$B$2</f>
         <v>Select Application Layer</v>
       </c>
-      <c r="E2" s="151"/>
-      <c r="F2" s="151"/>
-      <c r="G2" s="151"/>
-      <c r="H2" s="151"/>
-      <c r="I2" s="151"/>
-      <c r="J2" s="152"/>
-      <c r="L2" s="151" t="str">
+      <c r="E2" s="148"/>
+      <c r="F2" s="148"/>
+      <c r="G2" s="148"/>
+      <c r="H2" s="148"/>
+      <c r="I2" s="148"/>
+      <c r="J2" s="149"/>
+      <c r="L2" s="148" t="str">
         <f>'Knowledge Base'!$B$9</f>
         <v>Select Application Tier</v>
       </c>
-      <c r="M2" s="151"/>
-      <c r="N2" s="151"/>
-      <c r="O2" s="151"/>
-      <c r="P2" s="151"/>
-      <c r="Q2" s="151"/>
-      <c r="R2" s="152"/>
-      <c r="T2" s="151" t="str">
+      <c r="M2" s="148"/>
+      <c r="N2" s="148"/>
+      <c r="O2" s="148"/>
+      <c r="P2" s="148"/>
+      <c r="Q2" s="148"/>
+      <c r="R2" s="149"/>
+      <c r="T2" s="148" t="str">
         <f>'Knowledge Base'!$B$16</f>
         <v>Select Application Components</v>
       </c>
-      <c r="U2" s="151"/>
-      <c r="V2" s="151"/>
-      <c r="W2" s="151"/>
-      <c r="X2" s="151"/>
-      <c r="Y2" s="151"/>
-      <c r="Z2" s="151"/>
-      <c r="AA2" s="152"/>
-      <c r="AC2" s="151" t="str">
+      <c r="U2" s="148"/>
+      <c r="V2" s="148"/>
+      <c r="W2" s="148"/>
+      <c r="X2" s="148"/>
+      <c r="Y2" s="148"/>
+      <c r="Z2" s="148"/>
+      <c r="AA2" s="149"/>
+      <c r="AC2" s="148" t="str">
         <f>'Knowledge Base'!$B$24</f>
         <v>Select Migration Type</v>
       </c>
-      <c r="AD2" s="151"/>
-      <c r="AE2" s="151"/>
-      <c r="AF2" s="152"/>
-      <c r="AH2" s="151" t="str">
+      <c r="AD2" s="148"/>
+      <c r="AE2" s="148"/>
+      <c r="AF2" s="149"/>
+      <c r="AH2" s="148" t="str">
         <f>'Knowledge Base'!$B$28</f>
         <v>Define Scalability Level</v>
       </c>
-      <c r="AI2" s="151"/>
-      <c r="AJ2" s="151"/>
-      <c r="AK2" s="151"/>
-      <c r="AL2" s="151"/>
-      <c r="AM2" s="151"/>
-      <c r="AN2" s="151"/>
-      <c r="AO2" s="152"/>
-      <c r="AQ2" s="151" t="str">
+      <c r="AI2" s="148"/>
+      <c r="AJ2" s="148"/>
+      <c r="AK2" s="148"/>
+      <c r="AL2" s="148"/>
+      <c r="AM2" s="148"/>
+      <c r="AN2" s="148"/>
+      <c r="AO2" s="149"/>
+      <c r="AQ2" s="148" t="str">
         <f>'Knowledge Base'!$B$36</f>
         <v>Select Scaling Type</v>
       </c>
-      <c r="AR2" s="151"/>
-      <c r="AS2" s="152"/>
-      <c r="AU2" s="151" t="str">
+      <c r="AR2" s="148"/>
+      <c r="AS2" s="149"/>
+      <c r="AU2" s="148" t="str">
         <f>'Knowledge Base'!$B$39</f>
         <v>Select Elasticity Automation Degree</v>
       </c>
-      <c r="AV2" s="151"/>
-      <c r="AW2" s="151"/>
-      <c r="AX2" s="151"/>
-      <c r="AY2" s="152"/>
-      <c r="BA2" s="151" t="str">
+      <c r="AV2" s="148"/>
+      <c r="AW2" s="148"/>
+      <c r="AX2" s="148"/>
+      <c r="AY2" s="149"/>
+      <c r="BA2" s="148" t="str">
         <f>'Knowledge Base'!$B$44</f>
         <v>Select Scaling Trigger</v>
       </c>
-      <c r="BB2" s="151"/>
-      <c r="BC2" s="152"/>
-      <c r="BE2" s="151" t="str">
+      <c r="BB2" s="148"/>
+      <c r="BC2" s="149"/>
+      <c r="BE2" s="148" t="str">
         <f>'Knowledge Base'!$B$47</f>
         <v>Select Multi-Tenancy Level</v>
       </c>
-      <c r="BF2" s="151"/>
-      <c r="BG2" s="151"/>
-      <c r="BH2" s="152"/>
-      <c r="BJ2" s="151" t="str">
+      <c r="BF2" s="148"/>
+      <c r="BG2" s="148"/>
+      <c r="BH2" s="149"/>
+      <c r="BJ2" s="148" t="str">
         <f>'Knowledge Base'!$B$51</f>
         <v>Select Cloud Deployment Model</v>
       </c>
-      <c r="BK2" s="151"/>
-      <c r="BL2" s="151"/>
-      <c r="BM2" s="152"/>
-      <c r="BO2" s="151" t="str">
+      <c r="BK2" s="148"/>
+      <c r="BL2" s="148"/>
+      <c r="BM2" s="149"/>
+      <c r="BO2" s="148" t="str">
         <f>'Knowledge Base'!$B$55</f>
         <v>Select Cloud Service Model</v>
       </c>
-      <c r="BP2" s="151"/>
-      <c r="BQ2" s="151"/>
-      <c r="BR2" s="151"/>
-      <c r="BS2" s="151"/>
-      <c r="BT2" s="151"/>
-      <c r="BU2" s="152"/>
-      <c r="BW2" s="162" t="str">
+      <c r="BP2" s="148"/>
+      <c r="BQ2" s="148"/>
+      <c r="BR2" s="148"/>
+      <c r="BS2" s="148"/>
+      <c r="BT2" s="148"/>
+      <c r="BU2" s="149"/>
+      <c r="BW2" s="150" t="str">
         <f>'Knowledge Base'!$B$62</f>
         <v>Define Cloud Hosting</v>
       </c>
-      <c r="BX2" s="162"/>
-      <c r="BY2" s="163"/>
-      <c r="CA2" s="151" t="str">
+      <c r="BX2" s="150"/>
+      <c r="BY2" s="151"/>
+      <c r="CA2" s="148" t="str">
         <f>'Knowledge Base'!$B$65</f>
         <v>Define Roles of Responsibility</v>
       </c>
-      <c r="CB2" s="151"/>
-      <c r="CC2" s="151"/>
-      <c r="CD2" s="151"/>
-      <c r="CE2" s="151"/>
-      <c r="CF2" s="151"/>
-      <c r="CG2" s="152"/>
+      <c r="CB2" s="148"/>
+      <c r="CC2" s="148"/>
+      <c r="CD2" s="148"/>
+      <c r="CE2" s="148"/>
+      <c r="CF2" s="148"/>
+      <c r="CG2" s="149"/>
       <c r="CI2" s="118" t="str">
         <f>'Knowledge Base'!$B$72</f>
         <v>Select Cloud Vendor</v>
       </c>
-      <c r="CK2" s="151" t="str">
+      <c r="CK2" s="148" t="str">
         <f>'Knowledge Base'!$B$73</f>
         <v>Select Pricing Model</v>
       </c>
-      <c r="CL2" s="151"/>
-      <c r="CM2" s="151"/>
-      <c r="CN2" s="152"/>
-      <c r="CP2" s="151" t="str">
+      <c r="CL2" s="148"/>
+      <c r="CM2" s="148"/>
+      <c r="CN2" s="149"/>
+      <c r="CP2" s="148" t="str">
         <f>'Knowledge Base'!$B$77</f>
         <v>Define Resource Location</v>
       </c>
-      <c r="CQ2" s="152"/>
+      <c r="CQ2" s="149"/>
     </row>
     <row r="3" spans="1:98" s="7" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A3" s="24"/>
       <c r="B3" s="112"/>
-      <c r="C3" s="153" t="s">
+      <c r="C3" s="152" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="154"/>
-      <c r="E3" s="154"/>
-      <c r="F3" s="154"/>
-      <c r="G3" s="154"/>
-      <c r="H3" s="154"/>
-      <c r="I3" s="154"/>
-      <c r="J3" s="155"/>
+      <c r="D3" s="153"/>
+      <c r="E3" s="153"/>
+      <c r="F3" s="153"/>
+      <c r="G3" s="153"/>
+      <c r="H3" s="153"/>
+      <c r="I3" s="153"/>
+      <c r="J3" s="154"/>
       <c r="K3" s="11"/>
       <c r="L3" s="137" t="str">
         <f>'Decision Level'!$D$3</f>
@@ -8008,7 +7984,7 @@
       <c r="CQ3" s="138"/>
     </row>
     <row r="4" spans="1:98" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="150" t="str">
+      <c r="A4" s="161" t="str">
         <f>'Knowledge Base'!$B$2</f>
         <v>Select Application Layer</v>
       </c>
@@ -8016,14 +7992,14 @@
         <f>'Knowledge Base'!$C$2</f>
         <v>Presentation Layer</v>
       </c>
-      <c r="C4" s="156"/>
-      <c r="D4" s="157"/>
-      <c r="E4" s="157"/>
-      <c r="F4" s="157"/>
-      <c r="G4" s="157"/>
-      <c r="H4" s="157"/>
-      <c r="I4" s="157"/>
-      <c r="J4" s="158"/>
+      <c r="C4" s="155"/>
+      <c r="D4" s="156"/>
+      <c r="E4" s="156"/>
+      <c r="F4" s="156"/>
+      <c r="G4" s="156"/>
+      <c r="H4" s="156"/>
+      <c r="I4" s="156"/>
+      <c r="J4" s="157"/>
       <c r="K4" s="11"/>
       <c r="L4" s="11"/>
       <c r="M4" s="11"/>
@@ -8146,19 +8122,19 @@
       <c r="CT4" s="5"/>
     </row>
     <row r="5" spans="1:98" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="150"/>
+      <c r="A5" s="161"/>
       <c r="B5" s="113" t="str">
         <f>'Knowledge Base'!$C$3</f>
         <v>Business Layer</v>
       </c>
-      <c r="C5" s="156"/>
-      <c r="D5" s="157"/>
-      <c r="E5" s="157"/>
-      <c r="F5" s="157"/>
-      <c r="G5" s="157"/>
-      <c r="H5" s="157"/>
-      <c r="I5" s="157"/>
-      <c r="J5" s="158"/>
+      <c r="C5" s="155"/>
+      <c r="D5" s="156"/>
+      <c r="E5" s="156"/>
+      <c r="F5" s="156"/>
+      <c r="G5" s="156"/>
+      <c r="H5" s="156"/>
+      <c r="I5" s="156"/>
+      <c r="J5" s="157"/>
       <c r="K5" s="11"/>
       <c r="L5" s="11"/>
       <c r="M5" s="11"/>
@@ -8281,19 +8257,19 @@
       <c r="CT5" s="5"/>
     </row>
     <row r="6" spans="1:98" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="150"/>
+      <c r="A6" s="161"/>
       <c r="B6" s="113" t="str">
         <f>'Knowledge Base'!$C$4</f>
         <v>Resource Layer</v>
       </c>
-      <c r="C6" s="156"/>
-      <c r="D6" s="157"/>
-      <c r="E6" s="157"/>
-      <c r="F6" s="157"/>
-      <c r="G6" s="157"/>
-      <c r="H6" s="157"/>
-      <c r="I6" s="157"/>
-      <c r="J6" s="158"/>
+      <c r="C6" s="155"/>
+      <c r="D6" s="156"/>
+      <c r="E6" s="156"/>
+      <c r="F6" s="156"/>
+      <c r="G6" s="156"/>
+      <c r="H6" s="156"/>
+      <c r="I6" s="156"/>
+      <c r="J6" s="157"/>
       <c r="K6" s="11"/>
       <c r="L6" s="11"/>
       <c r="M6" s="11"/>
@@ -8416,19 +8392,19 @@
       <c r="CT6" s="5"/>
     </row>
     <row r="7" spans="1:98" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="150"/>
+      <c r="A7" s="161"/>
       <c r="B7" s="113" t="str">
         <f>'Knowledge Base'!$C$5</f>
         <v>Presentation + Business Layer</v>
       </c>
-      <c r="C7" s="156"/>
-      <c r="D7" s="157"/>
-      <c r="E7" s="157"/>
-      <c r="F7" s="157"/>
-      <c r="G7" s="157"/>
-      <c r="H7" s="157"/>
-      <c r="I7" s="157"/>
-      <c r="J7" s="158"/>
+      <c r="C7" s="155"/>
+      <c r="D7" s="156"/>
+      <c r="E7" s="156"/>
+      <c r="F7" s="156"/>
+      <c r="G7" s="156"/>
+      <c r="H7" s="156"/>
+      <c r="I7" s="156"/>
+      <c r="J7" s="157"/>
       <c r="K7" s="11"/>
       <c r="L7" s="11"/>
       <c r="M7" s="11"/>
@@ -8551,19 +8527,19 @@
       <c r="CT7" s="5"/>
     </row>
     <row r="8" spans="1:98" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="150"/>
+      <c r="A8" s="161"/>
       <c r="B8" s="113" t="str">
         <f>'Knowledge Base'!$C$6</f>
         <v>Presentation + Resource Layer</v>
       </c>
-      <c r="C8" s="156"/>
-      <c r="D8" s="157"/>
-      <c r="E8" s="157"/>
-      <c r="F8" s="157"/>
-      <c r="G8" s="157"/>
-      <c r="H8" s="157"/>
-      <c r="I8" s="157"/>
-      <c r="J8" s="158"/>
+      <c r="C8" s="155"/>
+      <c r="D8" s="156"/>
+      <c r="E8" s="156"/>
+      <c r="F8" s="156"/>
+      <c r="G8" s="156"/>
+      <c r="H8" s="156"/>
+      <c r="I8" s="156"/>
+      <c r="J8" s="157"/>
       <c r="K8" s="11"/>
       <c r="L8" s="11"/>
       <c r="M8" s="11"/>
@@ -8686,19 +8662,19 @@
       <c r="CT8" s="5"/>
     </row>
     <row r="9" spans="1:98" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="150"/>
+      <c r="A9" s="161"/>
       <c r="B9" s="113" t="str">
         <f>'Knowledge Base'!$C$7</f>
         <v>Business + Resource Layer</v>
       </c>
-      <c r="C9" s="156"/>
-      <c r="D9" s="157"/>
-      <c r="E9" s="157"/>
-      <c r="F9" s="157"/>
-      <c r="G9" s="157"/>
-      <c r="H9" s="157"/>
-      <c r="I9" s="157"/>
-      <c r="J9" s="158"/>
+      <c r="C9" s="155"/>
+      <c r="D9" s="156"/>
+      <c r="E9" s="156"/>
+      <c r="F9" s="156"/>
+      <c r="G9" s="156"/>
+      <c r="H9" s="156"/>
+      <c r="I9" s="156"/>
+      <c r="J9" s="157"/>
       <c r="K9" s="11"/>
       <c r="L9" s="11"/>
       <c r="M9" s="11"/>
@@ -8821,19 +8797,19 @@
       <c r="CT9" s="5"/>
     </row>
     <row r="10" spans="1:98" s="17" customFormat="1" ht="15" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="151"/>
+      <c r="A10" s="148"/>
       <c r="B10" s="114" t="str">
         <f>'Knowledge Base'!$C$8</f>
         <v>Presentation + Business + Resource Layer</v>
       </c>
-      <c r="C10" s="159"/>
-      <c r="D10" s="160"/>
-      <c r="E10" s="160"/>
-      <c r="F10" s="160"/>
-      <c r="G10" s="160"/>
-      <c r="H10" s="160"/>
-      <c r="I10" s="160"/>
-      <c r="J10" s="161"/>
+      <c r="C10" s="158"/>
+      <c r="D10" s="159"/>
+      <c r="E10" s="159"/>
+      <c r="F10" s="159"/>
+      <c r="G10" s="159"/>
+      <c r="H10" s="159"/>
+      <c r="I10" s="159"/>
+      <c r="J10" s="160"/>
       <c r="K10" s="35"/>
       <c r="L10" s="35"/>
       <c r="M10" s="35"/>
@@ -8969,16 +8945,16 @@
       <c r="H11" s="137"/>
       <c r="I11" s="137"/>
       <c r="J11" s="138"/>
-      <c r="K11" s="153" t="s">
+      <c r="K11" s="152" t="s">
         <v>41</v>
       </c>
-      <c r="L11" s="154"/>
-      <c r="M11" s="154"/>
-      <c r="N11" s="154"/>
-      <c r="O11" s="154"/>
-      <c r="P11" s="154"/>
-      <c r="Q11" s="154"/>
-      <c r="R11" s="155"/>
+      <c r="L11" s="153"/>
+      <c r="M11" s="153"/>
+      <c r="N11" s="153"/>
+      <c r="O11" s="153"/>
+      <c r="P11" s="153"/>
+      <c r="Q11" s="153"/>
+      <c r="R11" s="154"/>
       <c r="S11" s="11"/>
       <c r="T11" s="137" t="str">
         <f>'Decision Level'!$E$4</f>
@@ -9100,7 +9076,7 @@
       <c r="CQ11" s="138"/>
     </row>
     <row r="12" spans="1:98" s="5" customFormat="1" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="150" t="str">
+      <c r="A12" s="161" t="str">
         <f>'Knowledge Base'!$B$9</f>
         <v>Select Application Tier</v>
       </c>
@@ -9116,14 +9092,14 @@
       <c r="H12" s="13"/>
       <c r="I12" s="13"/>
       <c r="J12" s="14"/>
-      <c r="K12" s="156"/>
-      <c r="L12" s="157"/>
-      <c r="M12" s="157"/>
-      <c r="N12" s="157"/>
-      <c r="O12" s="157"/>
-      <c r="P12" s="157"/>
-      <c r="Q12" s="157"/>
-      <c r="R12" s="158"/>
+      <c r="K12" s="155"/>
+      <c r="L12" s="156"/>
+      <c r="M12" s="156"/>
+      <c r="N12" s="156"/>
+      <c r="O12" s="156"/>
+      <c r="P12" s="156"/>
+      <c r="Q12" s="156"/>
+      <c r="R12" s="157"/>
       <c r="S12" s="13"/>
       <c r="T12" s="13"/>
       <c r="U12" s="13"/>
@@ -9203,7 +9179,7 @@
       <c r="CQ12" s="12"/>
     </row>
     <row r="13" spans="1:98" s="5" customFormat="1" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="150"/>
+      <c r="A13" s="161"/>
       <c r="B13" s="112" t="str">
         <f>'Knowledge Base'!$C$10</f>
         <v>Application Tier</v>
@@ -9216,14 +9192,14 @@
       <c r="H13" s="13"/>
       <c r="I13" s="13"/>
       <c r="J13" s="14"/>
-      <c r="K13" s="156"/>
-      <c r="L13" s="157"/>
-      <c r="M13" s="157"/>
-      <c r="N13" s="157"/>
-      <c r="O13" s="157"/>
-      <c r="P13" s="157"/>
-      <c r="Q13" s="157"/>
-      <c r="R13" s="158"/>
+      <c r="K13" s="155"/>
+      <c r="L13" s="156"/>
+      <c r="M13" s="156"/>
+      <c r="N13" s="156"/>
+      <c r="O13" s="156"/>
+      <c r="P13" s="156"/>
+      <c r="Q13" s="156"/>
+      <c r="R13" s="157"/>
       <c r="S13" s="13"/>
       <c r="T13" s="13"/>
       <c r="U13" s="13"/>
@@ -9303,7 +9279,7 @@
       <c r="CQ13" s="12"/>
     </row>
     <row r="14" spans="1:98" s="5" customFormat="1" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="150"/>
+      <c r="A14" s="161"/>
       <c r="B14" s="112" t="str">
         <f>'Knowledge Base'!$C$11</f>
         <v>Data Tier</v>
@@ -9316,14 +9292,14 @@
       <c r="H14" s="13"/>
       <c r="I14" s="13"/>
       <c r="J14" s="14"/>
-      <c r="K14" s="156"/>
-      <c r="L14" s="157"/>
-      <c r="M14" s="157"/>
-      <c r="N14" s="157"/>
-      <c r="O14" s="157"/>
-      <c r="P14" s="157"/>
-      <c r="Q14" s="157"/>
-      <c r="R14" s="158"/>
+      <c r="K14" s="155"/>
+      <c r="L14" s="156"/>
+      <c r="M14" s="156"/>
+      <c r="N14" s="156"/>
+      <c r="O14" s="156"/>
+      <c r="P14" s="156"/>
+      <c r="Q14" s="156"/>
+      <c r="R14" s="157"/>
       <c r="S14" s="13"/>
       <c r="T14" s="13"/>
       <c r="U14" s="13"/>
@@ -9403,7 +9379,7 @@
       <c r="CQ14" s="12"/>
     </row>
     <row r="15" spans="1:98" s="5" customFormat="1" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="150"/>
+      <c r="A15" s="161"/>
       <c r="B15" s="112" t="str">
         <f>'Knowledge Base'!$C$12</f>
         <v>Client + Application Tier</v>
@@ -9416,14 +9392,14 @@
       <c r="H15" s="13"/>
       <c r="I15" s="13"/>
       <c r="J15" s="14"/>
-      <c r="K15" s="156"/>
-      <c r="L15" s="157"/>
-      <c r="M15" s="157"/>
-      <c r="N15" s="157"/>
-      <c r="O15" s="157"/>
-      <c r="P15" s="157"/>
-      <c r="Q15" s="157"/>
-      <c r="R15" s="158"/>
+      <c r="K15" s="155"/>
+      <c r="L15" s="156"/>
+      <c r="M15" s="156"/>
+      <c r="N15" s="156"/>
+      <c r="O15" s="156"/>
+      <c r="P15" s="156"/>
+      <c r="Q15" s="156"/>
+      <c r="R15" s="157"/>
       <c r="S15" s="13"/>
       <c r="T15" s="13"/>
       <c r="U15" s="13"/>
@@ -9503,7 +9479,7 @@
       <c r="CQ15" s="12"/>
     </row>
     <row r="16" spans="1:98" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="150"/>
+      <c r="A16" s="161"/>
       <c r="B16" s="113" t="str">
         <f>'Knowledge Base'!$C$13</f>
         <v>Client + Data Tier</v>
@@ -9516,14 +9492,14 @@
       <c r="H16" s="11"/>
       <c r="I16" s="11"/>
       <c r="J16" s="12"/>
-      <c r="K16" s="156"/>
-      <c r="L16" s="157"/>
-      <c r="M16" s="157"/>
-      <c r="N16" s="157"/>
-      <c r="O16" s="157"/>
-      <c r="P16" s="157"/>
-      <c r="Q16" s="157"/>
-      <c r="R16" s="158"/>
+      <c r="K16" s="155"/>
+      <c r="L16" s="156"/>
+      <c r="M16" s="156"/>
+      <c r="N16" s="156"/>
+      <c r="O16" s="156"/>
+      <c r="P16" s="156"/>
+      <c r="Q16" s="156"/>
+      <c r="R16" s="157"/>
       <c r="S16" s="11"/>
       <c r="T16" s="11"/>
       <c r="U16" s="11"/>
@@ -9606,7 +9582,7 @@
       <c r="CT16" s="5"/>
     </row>
     <row r="17" spans="1:98" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="150"/>
+      <c r="A17" s="161"/>
       <c r="B17" s="113" t="str">
         <f>'Knowledge Base'!$C$14</f>
         <v>Application + Data Tier</v>
@@ -9619,14 +9595,14 @@
       <c r="H17" s="11"/>
       <c r="I17" s="11"/>
       <c r="J17" s="12"/>
-      <c r="K17" s="156"/>
-      <c r="L17" s="157"/>
-      <c r="M17" s="157"/>
-      <c r="N17" s="157"/>
-      <c r="O17" s="157"/>
-      <c r="P17" s="157"/>
-      <c r="Q17" s="157"/>
-      <c r="R17" s="158"/>
+      <c r="K17" s="155"/>
+      <c r="L17" s="156"/>
+      <c r="M17" s="156"/>
+      <c r="N17" s="156"/>
+      <c r="O17" s="156"/>
+      <c r="P17" s="156"/>
+      <c r="Q17" s="156"/>
+      <c r="R17" s="157"/>
       <c r="S17" s="11"/>
       <c r="T17" s="11"/>
       <c r="U17" s="11"/>
@@ -9709,7 +9685,7 @@
       <c r="CT17" s="5"/>
     </row>
     <row r="18" spans="1:98" s="17" customFormat="1" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="151"/>
+      <c r="A18" s="148"/>
       <c r="B18" s="114" t="str">
         <f>'Knowledge Base'!$C$15</f>
         <v>Client + Application + Data Tier</v>
@@ -9722,14 +9698,14 @@
       <c r="H18" s="35"/>
       <c r="I18" s="35"/>
       <c r="J18" s="36"/>
-      <c r="K18" s="159"/>
-      <c r="L18" s="160"/>
-      <c r="M18" s="160"/>
-      <c r="N18" s="160"/>
-      <c r="O18" s="160"/>
-      <c r="P18" s="160"/>
-      <c r="Q18" s="160"/>
-      <c r="R18" s="161"/>
+      <c r="K18" s="158"/>
+      <c r="L18" s="159"/>
+      <c r="M18" s="159"/>
+      <c r="N18" s="159"/>
+      <c r="O18" s="159"/>
+      <c r="P18" s="159"/>
+      <c r="Q18" s="159"/>
+      <c r="R18" s="160"/>
       <c r="S18" s="35"/>
       <c r="T18" s="35"/>
       <c r="U18" s="35"/>
@@ -9836,17 +9812,17 @@
       <c r="P19" s="137"/>
       <c r="Q19" s="137"/>
       <c r="R19" s="138"/>
-      <c r="S19" s="153" t="s">
+      <c r="S19" s="152" t="s">
         <v>41</v>
       </c>
-      <c r="T19" s="154"/>
-      <c r="U19" s="154"/>
-      <c r="V19" s="154"/>
-      <c r="W19" s="154"/>
-      <c r="X19" s="154"/>
-      <c r="Y19" s="154"/>
-      <c r="Z19" s="154"/>
-      <c r="AA19" s="155"/>
+      <c r="T19" s="153"/>
+      <c r="U19" s="153"/>
+      <c r="V19" s="153"/>
+      <c r="W19" s="153"/>
+      <c r="X19" s="153"/>
+      <c r="Y19" s="153"/>
+      <c r="Z19" s="153"/>
+      <c r="AA19" s="154"/>
       <c r="AB19" s="11"/>
       <c r="AC19" s="137" t="str">
         <f>'Decision Level'!$F$5</f>
@@ -9956,7 +9932,7 @@
       <c r="CQ19" s="138"/>
     </row>
     <row r="20" spans="1:98" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="150" t="str">
+      <c r="A20" s="161" t="str">
         <f>'Knowledge Base'!$B$16</f>
         <v>Select Application Components</v>
       </c>
@@ -9994,15 +9970,15 @@
       <c r="P20" s="11"/>
       <c r="Q20" s="11"/>
       <c r="R20" s="12"/>
-      <c r="S20" s="156"/>
-      <c r="T20" s="157"/>
-      <c r="U20" s="157"/>
-      <c r="V20" s="157"/>
-      <c r="W20" s="157"/>
-      <c r="X20" s="157"/>
-      <c r="Y20" s="157"/>
-      <c r="Z20" s="157"/>
-      <c r="AA20" s="158"/>
+      <c r="S20" s="155"/>
+      <c r="T20" s="156"/>
+      <c r="U20" s="156"/>
+      <c r="V20" s="156"/>
+      <c r="W20" s="156"/>
+      <c r="X20" s="156"/>
+      <c r="Y20" s="156"/>
+      <c r="Z20" s="156"/>
+      <c r="AA20" s="157"/>
       <c r="AB20" s="11"/>
       <c r="AC20" s="11" t="s">
         <v>86</v>
@@ -10122,7 +10098,7 @@
       <c r="CT20" s="5"/>
     </row>
     <row r="21" spans="1:98" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="150"/>
+      <c r="A21" s="161"/>
       <c r="B21" s="113" t="str">
         <f>'Knowledge Base'!$C$17</f>
         <v>Application Components</v>
@@ -10157,15 +10133,15 @@
       <c r="P21" s="11"/>
       <c r="Q21" s="11"/>
       <c r="R21" s="12"/>
-      <c r="S21" s="156"/>
-      <c r="T21" s="157"/>
-      <c r="U21" s="157"/>
-      <c r="V21" s="157"/>
-      <c r="W21" s="157"/>
-      <c r="X21" s="157"/>
-      <c r="Y21" s="157"/>
-      <c r="Z21" s="157"/>
-      <c r="AA21" s="158"/>
+      <c r="S21" s="155"/>
+      <c r="T21" s="156"/>
+      <c r="U21" s="156"/>
+      <c r="V21" s="156"/>
+      <c r="W21" s="156"/>
+      <c r="X21" s="156"/>
+      <c r="Y21" s="156"/>
+      <c r="Z21" s="156"/>
+      <c r="AA21" s="157"/>
       <c r="AB21" s="15"/>
       <c r="AC21" s="11" t="s">
         <v>87</v>
@@ -10285,7 +10261,7 @@
       <c r="CT21" s="5"/>
     </row>
     <row r="22" spans="1:98" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="150"/>
+      <c r="A22" s="161"/>
       <c r="B22" s="113" t="str">
         <f>'Knowledge Base'!$C$18</f>
         <v>Middleware Component</v>
@@ -10320,15 +10296,15 @@
       <c r="P22" s="11"/>
       <c r="Q22" s="11"/>
       <c r="R22" s="12"/>
-      <c r="S22" s="156"/>
-      <c r="T22" s="157"/>
-      <c r="U22" s="157"/>
-      <c r="V22" s="157"/>
-      <c r="W22" s="157"/>
-      <c r="X22" s="157"/>
-      <c r="Y22" s="157"/>
-      <c r="Z22" s="157"/>
-      <c r="AA22" s="158"/>
+      <c r="S22" s="155"/>
+      <c r="T22" s="156"/>
+      <c r="U22" s="156"/>
+      <c r="V22" s="156"/>
+      <c r="W22" s="156"/>
+      <c r="X22" s="156"/>
+      <c r="Y22" s="156"/>
+      <c r="Z22" s="156"/>
+      <c r="AA22" s="157"/>
       <c r="AB22" s="15"/>
       <c r="AC22" s="11" t="s">
         <v>86</v>
@@ -10448,7 +10424,7 @@
       <c r="CT22" s="5"/>
     </row>
     <row r="23" spans="1:98" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="150"/>
+      <c r="A23" s="161"/>
       <c r="B23" s="113" t="str">
         <f>'Knowledge Base'!$C$19</f>
         <v>Middleware Components</v>
@@ -10483,15 +10459,15 @@
       <c r="P23" s="11"/>
       <c r="Q23" s="11"/>
       <c r="R23" s="12"/>
-      <c r="S23" s="156"/>
-      <c r="T23" s="157"/>
-      <c r="U23" s="157"/>
-      <c r="V23" s="157"/>
-      <c r="W23" s="157"/>
-      <c r="X23" s="157"/>
-      <c r="Y23" s="157"/>
-      <c r="Z23" s="157"/>
-      <c r="AA23" s="158"/>
+      <c r="S23" s="155"/>
+      <c r="T23" s="156"/>
+      <c r="U23" s="156"/>
+      <c r="V23" s="156"/>
+      <c r="W23" s="156"/>
+      <c r="X23" s="156"/>
+      <c r="Y23" s="156"/>
+      <c r="Z23" s="156"/>
+      <c r="AA23" s="157"/>
       <c r="AB23" s="15"/>
       <c r="AC23" s="11" t="s">
         <v>87</v>
@@ -10611,7 +10587,7 @@
       <c r="CT23" s="5"/>
     </row>
     <row r="24" spans="1:98" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="150"/>
+      <c r="A24" s="161"/>
       <c r="B24" s="113" t="str">
         <f>'Knowledge Base'!$C$20</f>
         <v>Application + Middleware Component</v>
@@ -10646,15 +10622,15 @@
       <c r="P24" s="11"/>
       <c r="Q24" s="11"/>
       <c r="R24" s="12"/>
-      <c r="S24" s="156"/>
-      <c r="T24" s="157"/>
-      <c r="U24" s="157"/>
-      <c r="V24" s="157"/>
-      <c r="W24" s="157"/>
-      <c r="X24" s="157"/>
-      <c r="Y24" s="157"/>
-      <c r="Z24" s="157"/>
-      <c r="AA24" s="158"/>
+      <c r="S24" s="155"/>
+      <c r="T24" s="156"/>
+      <c r="U24" s="156"/>
+      <c r="V24" s="156"/>
+      <c r="W24" s="156"/>
+      <c r="X24" s="156"/>
+      <c r="Y24" s="156"/>
+      <c r="Z24" s="156"/>
+      <c r="AA24" s="157"/>
       <c r="AB24" s="15"/>
       <c r="AC24" s="11" t="s">
         <v>87</v>
@@ -10774,7 +10750,7 @@
       <c r="CT24" s="5"/>
     </row>
     <row r="25" spans="1:98" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="150"/>
+      <c r="A25" s="161"/>
       <c r="B25" s="113" t="str">
         <f>'Knowledge Base'!$C$21</f>
         <v>Application Component + Middleware Components</v>
@@ -10809,15 +10785,15 @@
       <c r="P25" s="11"/>
       <c r="Q25" s="11"/>
       <c r="R25" s="12"/>
-      <c r="S25" s="156"/>
-      <c r="T25" s="157"/>
-      <c r="U25" s="157"/>
-      <c r="V25" s="157"/>
-      <c r="W25" s="157"/>
-      <c r="X25" s="157"/>
-      <c r="Y25" s="157"/>
-      <c r="Z25" s="157"/>
-      <c r="AA25" s="158"/>
+      <c r="S25" s="155"/>
+      <c r="T25" s="156"/>
+      <c r="U25" s="156"/>
+      <c r="V25" s="156"/>
+      <c r="W25" s="156"/>
+      <c r="X25" s="156"/>
+      <c r="Y25" s="156"/>
+      <c r="Z25" s="156"/>
+      <c r="AA25" s="157"/>
       <c r="AB25" s="11"/>
       <c r="AC25" s="11" t="s">
         <v>87</v>
@@ -10937,7 +10913,7 @@
       <c r="CT25" s="5"/>
     </row>
     <row r="26" spans="1:98" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="150"/>
+      <c r="A26" s="161"/>
       <c r="B26" s="113" t="str">
         <f>'Knowledge Base'!$C$22</f>
         <v>Middleware Component + Application Components</v>
@@ -10972,15 +10948,15 @@
       <c r="P26" s="11"/>
       <c r="Q26" s="11"/>
       <c r="R26" s="12"/>
-      <c r="S26" s="156"/>
-      <c r="T26" s="157"/>
-      <c r="U26" s="157"/>
-      <c r="V26" s="157"/>
-      <c r="W26" s="157"/>
-      <c r="X26" s="157"/>
-      <c r="Y26" s="157"/>
-      <c r="Z26" s="157"/>
-      <c r="AA26" s="158"/>
+      <c r="S26" s="155"/>
+      <c r="T26" s="156"/>
+      <c r="U26" s="156"/>
+      <c r="V26" s="156"/>
+      <c r="W26" s="156"/>
+      <c r="X26" s="156"/>
+      <c r="Y26" s="156"/>
+      <c r="Z26" s="156"/>
+      <c r="AA26" s="157"/>
       <c r="AB26" s="15"/>
       <c r="AC26" s="11" t="s">
         <v>87</v>
@@ -11100,7 +11076,7 @@
       <c r="CT26" s="5"/>
     </row>
     <row r="27" spans="1:98" s="18" customFormat="1" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="151"/>
+      <c r="A27" s="148"/>
       <c r="B27" s="115" t="str">
         <f>'Knowledge Base'!$C$23</f>
         <v>Application + Middleware Components</v>
@@ -11135,15 +11111,15 @@
       <c r="P27" s="35"/>
       <c r="Q27" s="35"/>
       <c r="R27" s="36"/>
-      <c r="S27" s="159"/>
-      <c r="T27" s="160"/>
-      <c r="U27" s="160"/>
-      <c r="V27" s="160"/>
-      <c r="W27" s="160"/>
-      <c r="X27" s="160"/>
-      <c r="Y27" s="160"/>
-      <c r="Z27" s="160"/>
-      <c r="AA27" s="161"/>
+      <c r="S27" s="158"/>
+      <c r="T27" s="159"/>
+      <c r="U27" s="159"/>
+      <c r="V27" s="159"/>
+      <c r="W27" s="159"/>
+      <c r="X27" s="159"/>
+      <c r="Y27" s="159"/>
+      <c r="Z27" s="159"/>
+      <c r="AA27" s="160"/>
       <c r="AB27" s="35"/>
       <c r="AC27" s="35" t="s">
         <v>87</v>
@@ -11299,13 +11275,13 @@
       <c r="Y28" s="137"/>
       <c r="Z28" s="137"/>
       <c r="AA28" s="138"/>
-      <c r="AB28" s="153" t="s">
+      <c r="AB28" s="152" t="s">
         <v>41</v>
       </c>
-      <c r="AC28" s="154"/>
-      <c r="AD28" s="154"/>
-      <c r="AE28" s="154"/>
-      <c r="AF28" s="155"/>
+      <c r="AC28" s="153"/>
+      <c r="AD28" s="153"/>
+      <c r="AE28" s="153"/>
+      <c r="AF28" s="154"/>
       <c r="AG28" s="11"/>
       <c r="AH28" s="137" t="str">
         <f>'Decision Level'!G6</f>
@@ -11407,7 +11383,7 @@
       <c r="CQ28" s="138"/>
     </row>
     <row r="29" spans="1:98" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="150" t="str">
+      <c r="A29" s="161" t="str">
         <f>'Knowledge Base'!$B$24</f>
         <v>Select Migration Type</v>
       </c>
@@ -11470,11 +11446,11 @@
       <c r="AA29" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AB29" s="156"/>
-      <c r="AC29" s="157"/>
-      <c r="AD29" s="157"/>
-      <c r="AE29" s="157"/>
-      <c r="AF29" s="158"/>
+      <c r="AB29" s="155"/>
+      <c r="AC29" s="156"/>
+      <c r="AD29" s="156"/>
+      <c r="AE29" s="156"/>
+      <c r="AF29" s="157"/>
       <c r="AG29" s="11"/>
       <c r="AH29" s="11" t="s">
         <v>86</v>
@@ -11581,7 +11557,7 @@
       <c r="CT29" s="5"/>
     </row>
     <row r="30" spans="1:98" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="150"/>
+      <c r="A30" s="161"/>
       <c r="B30" s="113" t="str">
         <f>'Knowledge Base'!$C$25</f>
         <v>Migration Type II</v>
@@ -11641,11 +11617,11 @@
       <c r="AA30" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="AB30" s="156"/>
-      <c r="AC30" s="157"/>
-      <c r="AD30" s="157"/>
-      <c r="AE30" s="157"/>
-      <c r="AF30" s="158"/>
+      <c r="AB30" s="155"/>
+      <c r="AC30" s="156"/>
+      <c r="AD30" s="156"/>
+      <c r="AE30" s="156"/>
+      <c r="AF30" s="157"/>
       <c r="AG30" s="11"/>
       <c r="AH30" s="11" t="s">
         <v>86</v>
@@ -11752,7 +11728,7 @@
       <c r="CT30" s="5"/>
     </row>
     <row r="31" spans="1:98" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="150"/>
+      <c r="A31" s="161"/>
       <c r="B31" s="113" t="str">
         <f>'Knowledge Base'!$C$26</f>
         <v>Migration Type III</v>
@@ -11812,11 +11788,11 @@
       <c r="AA31" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="AB31" s="156"/>
-      <c r="AC31" s="157"/>
-      <c r="AD31" s="157"/>
-      <c r="AE31" s="157"/>
-      <c r="AF31" s="158"/>
+      <c r="AB31" s="155"/>
+      <c r="AC31" s="156"/>
+      <c r="AD31" s="156"/>
+      <c r="AE31" s="156"/>
+      <c r="AF31" s="157"/>
       <c r="AG31" s="11"/>
       <c r="AH31" s="11" t="s">
         <v>86</v>
@@ -11923,7 +11899,7 @@
       <c r="CT31" s="5"/>
     </row>
     <row r="32" spans="1:98" s="19" customFormat="1" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="151"/>
+      <c r="A32" s="148"/>
       <c r="B32" s="115" t="str">
         <f>'Knowledge Base'!$C$27</f>
         <v>Migration Type IV</v>
@@ -11983,11 +11959,11 @@
       <c r="AA32" s="36" t="s">
         <v>85</v>
       </c>
-      <c r="AB32" s="159"/>
-      <c r="AC32" s="160"/>
-      <c r="AD32" s="160"/>
-      <c r="AE32" s="160"/>
-      <c r="AF32" s="161"/>
+      <c r="AB32" s="158"/>
+      <c r="AC32" s="159"/>
+      <c r="AD32" s="159"/>
+      <c r="AE32" s="159"/>
+      <c r="AF32" s="160"/>
       <c r="AG32" s="35"/>
       <c r="AH32" s="35" t="s">
         <v>87</v>
@@ -12138,14 +12114,14 @@
       <c r="AG33" s="139" t="s">
         <v>41</v>
       </c>
-      <c r="AH33" s="140"/>
-      <c r="AI33" s="140"/>
-      <c r="AJ33" s="140"/>
-      <c r="AK33" s="140"/>
-      <c r="AL33" s="140"/>
-      <c r="AM33" s="140"/>
-      <c r="AN33" s="140"/>
-      <c r="AO33" s="141"/>
+      <c r="AH33" s="143"/>
+      <c r="AI33" s="143"/>
+      <c r="AJ33" s="143"/>
+      <c r="AK33" s="143"/>
+      <c r="AL33" s="143"/>
+      <c r="AM33" s="143"/>
+      <c r="AN33" s="143"/>
+      <c r="AO33" s="140"/>
       <c r="AP33" s="59"/>
       <c r="AQ33" s="137" t="str">
         <f>'Decision Level'!H7</f>
@@ -12238,7 +12214,7 @@
       <c r="CT33" s="5"/>
     </row>
     <row r="34" spans="1:98" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="150" t="str">
+      <c r="A34" s="161" t="str">
         <f>'Knowledge Base'!$B$28</f>
         <v>Define Scalability Level</v>
       </c>
@@ -12300,15 +12276,15 @@
       <c r="AF34" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AG34" s="142"/>
-      <c r="AH34" s="143"/>
-      <c r="AI34" s="143"/>
-      <c r="AJ34" s="143"/>
-      <c r="AK34" s="143"/>
-      <c r="AL34" s="143"/>
-      <c r="AM34" s="143"/>
-      <c r="AN34" s="143"/>
-      <c r="AO34" s="144"/>
+      <c r="AG34" s="144"/>
+      <c r="AH34" s="145"/>
+      <c r="AI34" s="145"/>
+      <c r="AJ34" s="145"/>
+      <c r="AK34" s="145"/>
+      <c r="AL34" s="145"/>
+      <c r="AM34" s="145"/>
+      <c r="AN34" s="145"/>
+      <c r="AO34" s="146"/>
       <c r="AP34" s="11"/>
       <c r="AQ34" s="11" t="s">
         <v>87</v>
@@ -12414,7 +12390,7 @@
       <c r="CT34" s="5"/>
     </row>
     <row r="35" spans="1:98" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="150"/>
+      <c r="A35" s="161"/>
       <c r="B35" s="113" t="str">
         <f>'Knowledge Base'!$C$29</f>
         <v>VM Level Scaling</v>
@@ -12473,15 +12449,15 @@
       <c r="AF35" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="AG35" s="142"/>
-      <c r="AH35" s="143"/>
-      <c r="AI35" s="143"/>
-      <c r="AJ35" s="143"/>
-      <c r="AK35" s="143"/>
-      <c r="AL35" s="143"/>
-      <c r="AM35" s="143"/>
-      <c r="AN35" s="143"/>
-      <c r="AO35" s="144"/>
+      <c r="AG35" s="144"/>
+      <c r="AH35" s="145"/>
+      <c r="AI35" s="145"/>
+      <c r="AJ35" s="145"/>
+      <c r="AK35" s="145"/>
+      <c r="AL35" s="145"/>
+      <c r="AM35" s="145"/>
+      <c r="AN35" s="145"/>
+      <c r="AO35" s="146"/>
       <c r="AP35" s="11"/>
       <c r="AQ35" s="11" t="s">
         <v>86</v>
@@ -12587,7 +12563,7 @@
       <c r="CT35" s="5"/>
     </row>
     <row r="36" spans="1:98" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="150"/>
+      <c r="A36" s="161"/>
       <c r="B36" s="113" t="str">
         <f>'Knowledge Base'!$C$30</f>
         <v>Middleware Level Scaling</v>
@@ -12646,15 +12622,15 @@
       <c r="AF36" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="AG36" s="142"/>
-      <c r="AH36" s="143"/>
-      <c r="AI36" s="143"/>
-      <c r="AJ36" s="143"/>
-      <c r="AK36" s="143"/>
-      <c r="AL36" s="143"/>
-      <c r="AM36" s="143"/>
-      <c r="AN36" s="143"/>
-      <c r="AO36" s="144"/>
+      <c r="AG36" s="144"/>
+      <c r="AH36" s="145"/>
+      <c r="AI36" s="145"/>
+      <c r="AJ36" s="145"/>
+      <c r="AK36" s="145"/>
+      <c r="AL36" s="145"/>
+      <c r="AM36" s="145"/>
+      <c r="AN36" s="145"/>
+      <c r="AO36" s="146"/>
       <c r="AP36" s="11"/>
       <c r="AQ36" s="11" t="s">
         <v>87</v>
@@ -12760,7 +12736,7 @@
       <c r="CT36" s="5"/>
     </row>
     <row r="37" spans="1:98" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="150"/>
+      <c r="A37" s="161"/>
       <c r="B37" s="113" t="str">
         <f>'Knowledge Base'!$C$31</f>
         <v>Application Level Scaling</v>
@@ -12819,15 +12795,15 @@
       <c r="AF37" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="AG37" s="142"/>
-      <c r="AH37" s="143"/>
-      <c r="AI37" s="143"/>
-      <c r="AJ37" s="143"/>
-      <c r="AK37" s="143"/>
-      <c r="AL37" s="143"/>
-      <c r="AM37" s="143"/>
-      <c r="AN37" s="143"/>
-      <c r="AO37" s="144"/>
+      <c r="AG37" s="144"/>
+      <c r="AH37" s="145"/>
+      <c r="AI37" s="145"/>
+      <c r="AJ37" s="145"/>
+      <c r="AK37" s="145"/>
+      <c r="AL37" s="145"/>
+      <c r="AM37" s="145"/>
+      <c r="AN37" s="145"/>
+      <c r="AO37" s="146"/>
       <c r="AP37" s="11"/>
       <c r="AQ37" s="11" t="s">
         <v>87</v>
@@ -12933,7 +12909,7 @@
       <c r="CT37" s="5"/>
     </row>
     <row r="38" spans="1:98" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="150"/>
+      <c r="A38" s="161"/>
       <c r="B38" s="113" t="str">
         <f>'Knowledge Base'!$C$32</f>
         <v>VM + Middleware Level Scaling</v>
@@ -12992,15 +12968,15 @@
       <c r="AF38" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="AG38" s="142"/>
-      <c r="AH38" s="143"/>
-      <c r="AI38" s="143"/>
-      <c r="AJ38" s="143"/>
-      <c r="AK38" s="143"/>
-      <c r="AL38" s="143"/>
-      <c r="AM38" s="143"/>
-      <c r="AN38" s="143"/>
-      <c r="AO38" s="144"/>
+      <c r="AG38" s="144"/>
+      <c r="AH38" s="145"/>
+      <c r="AI38" s="145"/>
+      <c r="AJ38" s="145"/>
+      <c r="AK38" s="145"/>
+      <c r="AL38" s="145"/>
+      <c r="AM38" s="145"/>
+      <c r="AN38" s="145"/>
+      <c r="AO38" s="146"/>
       <c r="AP38" s="11"/>
       <c r="AQ38" s="11" t="s">
         <v>87</v>
@@ -13106,7 +13082,7 @@
       <c r="CT38" s="5"/>
     </row>
     <row r="39" spans="1:98" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="150"/>
+      <c r="A39" s="161"/>
       <c r="B39" s="113" t="str">
         <f>'Knowledge Base'!$C$33</f>
         <v>VM + Application Level Scaling</v>
@@ -13165,15 +13141,15 @@
       <c r="AF39" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="AG39" s="142"/>
-      <c r="AH39" s="143"/>
-      <c r="AI39" s="143"/>
-      <c r="AJ39" s="143"/>
-      <c r="AK39" s="143"/>
-      <c r="AL39" s="143"/>
-      <c r="AM39" s="143"/>
-      <c r="AN39" s="143"/>
-      <c r="AO39" s="144"/>
+      <c r="AG39" s="144"/>
+      <c r="AH39" s="145"/>
+      <c r="AI39" s="145"/>
+      <c r="AJ39" s="145"/>
+      <c r="AK39" s="145"/>
+      <c r="AL39" s="145"/>
+      <c r="AM39" s="145"/>
+      <c r="AN39" s="145"/>
+      <c r="AO39" s="146"/>
       <c r="AP39" s="11"/>
       <c r="AQ39" s="11" t="s">
         <v>87</v>
@@ -13279,7 +13255,7 @@
       <c r="CT39" s="5"/>
     </row>
     <row r="40" spans="1:98" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="150"/>
+      <c r="A40" s="161"/>
       <c r="B40" s="113" t="str">
         <f>'Knowledge Base'!$C$34</f>
         <v>Middleware + Application Level Scaling</v>
@@ -13338,15 +13314,15 @@
       <c r="AF40" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="AG40" s="142"/>
-      <c r="AH40" s="143"/>
-      <c r="AI40" s="143"/>
-      <c r="AJ40" s="143"/>
-      <c r="AK40" s="143"/>
-      <c r="AL40" s="143"/>
-      <c r="AM40" s="143"/>
-      <c r="AN40" s="143"/>
-      <c r="AO40" s="144"/>
+      <c r="AG40" s="144"/>
+      <c r="AH40" s="145"/>
+      <c r="AI40" s="145"/>
+      <c r="AJ40" s="145"/>
+      <c r="AK40" s="145"/>
+      <c r="AL40" s="145"/>
+      <c r="AM40" s="145"/>
+      <c r="AN40" s="145"/>
+      <c r="AO40" s="146"/>
       <c r="AP40" s="11"/>
       <c r="AQ40" s="11" t="s">
         <v>87</v>
@@ -13452,7 +13428,7 @@
       <c r="CT40" s="5"/>
     </row>
     <row r="41" spans="1:98" s="19" customFormat="1" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="151"/>
+      <c r="A41" s="148"/>
       <c r="B41" s="115" t="str">
         <f>'Knowledge Base'!$C$35</f>
         <v>VM + Middleware + Application Level Scaling</v>
@@ -13511,15 +13487,15 @@
       <c r="AF41" s="36" t="s">
         <v>86</v>
       </c>
-      <c r="AG41" s="145"/>
-      <c r="AH41" s="146"/>
-      <c r="AI41" s="146"/>
-      <c r="AJ41" s="146"/>
-      <c r="AK41" s="146"/>
-      <c r="AL41" s="146"/>
-      <c r="AM41" s="146"/>
-      <c r="AN41" s="146"/>
-      <c r="AO41" s="147"/>
+      <c r="AG41" s="141"/>
+      <c r="AH41" s="147"/>
+      <c r="AI41" s="147"/>
+      <c r="AJ41" s="147"/>
+      <c r="AK41" s="147"/>
+      <c r="AL41" s="147"/>
+      <c r="AM41" s="147"/>
+      <c r="AN41" s="147"/>
+      <c r="AO41" s="142"/>
       <c r="AP41" s="35"/>
       <c r="AQ41" s="35" t="s">
         <v>87</v>
@@ -13682,9 +13658,9 @@
       <c r="AP42" s="139" t="s">
         <v>41</v>
       </c>
-      <c r="AQ42" s="140"/>
-      <c r="AR42" s="140"/>
-      <c r="AS42" s="141"/>
+      <c r="AQ42" s="143"/>
+      <c r="AR42" s="143"/>
+      <c r="AS42" s="140"/>
       <c r="AT42" s="59"/>
       <c r="AU42" s="137" t="str">
         <f>'Decision Level'!I8</f>
@@ -13770,7 +13746,7 @@
       <c r="CT42" s="5"/>
     </row>
     <row r="43" spans="1:98" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="150" t="str">
+      <c r="A43" s="161" t="str">
         <f>'Knowledge Base'!$B$36</f>
         <v>Select Scaling Type</v>
       </c>
@@ -13833,10 +13809,10 @@
       <c r="AO43" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AP43" s="142"/>
-      <c r="AQ43" s="143"/>
-      <c r="AR43" s="143"/>
-      <c r="AS43" s="144"/>
+      <c r="AP43" s="144"/>
+      <c r="AQ43" s="145"/>
+      <c r="AR43" s="145"/>
+      <c r="AS43" s="146"/>
       <c r="AT43" s="11"/>
       <c r="AU43" s="11"/>
       <c r="AV43" s="11"/>
@@ -13908,7 +13884,7 @@
       <c r="CT43" s="5"/>
     </row>
     <row r="44" spans="1:98" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="150"/>
+      <c r="A44" s="161"/>
       <c r="B44" s="113" t="str">
         <f>'Knowledge Base'!$C$37</f>
         <v>Horizontal Scaling</v>
@@ -13967,10 +13943,10 @@
       <c r="AO44" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="AP44" s="142"/>
-      <c r="AQ44" s="143"/>
-      <c r="AR44" s="143"/>
-      <c r="AS44" s="144"/>
+      <c r="AP44" s="144"/>
+      <c r="AQ44" s="145"/>
+      <c r="AR44" s="145"/>
+      <c r="AS44" s="146"/>
       <c r="AT44" s="11"/>
       <c r="AU44" s="11"/>
       <c r="AV44" s="11"/>
@@ -14042,7 +14018,7 @@
       <c r="CT44" s="5"/>
     </row>
     <row r="45" spans="1:98" s="19" customFormat="1" ht="15" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="151"/>
+      <c r="A45" s="148"/>
       <c r="B45" s="115" t="str">
         <f>'Knowledge Base'!$C$38</f>
         <v>Hybrid Scaling</v>
@@ -14102,10 +14078,10 @@
       <c r="AO45" s="36" t="s">
         <v>86</v>
       </c>
-      <c r="AP45" s="145"/>
-      <c r="AQ45" s="146"/>
-      <c r="AR45" s="146"/>
-      <c r="AS45" s="147"/>
+      <c r="AP45" s="141"/>
+      <c r="AQ45" s="147"/>
+      <c r="AR45" s="147"/>
+      <c r="AS45" s="142"/>
       <c r="AT45" s="35"/>
       <c r="AU45" s="35"/>
       <c r="AV45" s="35"/>
@@ -14241,11 +14217,11 @@
       <c r="AT46" s="139" t="s">
         <v>41</v>
       </c>
-      <c r="AU46" s="140"/>
-      <c r="AV46" s="140"/>
-      <c r="AW46" s="140"/>
-      <c r="AX46" s="140"/>
-      <c r="AY46" s="141"/>
+      <c r="AU46" s="143"/>
+      <c r="AV46" s="143"/>
+      <c r="AW46" s="143"/>
+      <c r="AX46" s="143"/>
+      <c r="AY46" s="140"/>
       <c r="AZ46" s="11"/>
       <c r="BA46" s="137" t="str">
         <f>'Decision Level'!J9</f>
@@ -14322,7 +14298,7 @@
       <c r="CT46" s="5"/>
     </row>
     <row r="47" spans="1:98" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="150" t="str">
+      <c r="A47" s="161" t="str">
         <f>'Knowledge Base'!$B$39</f>
         <v>Select Elasticity Automation Degree</v>
       </c>
@@ -14389,12 +14365,12 @@
       <c r="AQ47" s="59"/>
       <c r="AR47" s="11"/>
       <c r="AS47" s="12"/>
-      <c r="AT47" s="142"/>
-      <c r="AU47" s="143"/>
-      <c r="AV47" s="143"/>
-      <c r="AW47" s="143"/>
-      <c r="AX47" s="143"/>
-      <c r="AY47" s="144"/>
+      <c r="AT47" s="144"/>
+      <c r="AU47" s="145"/>
+      <c r="AV47" s="145"/>
+      <c r="AW47" s="145"/>
+      <c r="AX47" s="145"/>
+      <c r="AY47" s="146"/>
       <c r="AZ47" s="11"/>
       <c r="BA47" s="11" t="s">
         <v>85</v>
@@ -14466,7 +14442,7 @@
       <c r="CT47" s="5"/>
     </row>
     <row r="48" spans="1:98" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="150"/>
+      <c r="A48" s="161"/>
       <c r="B48" s="113" t="str">
         <f>'Knowledge Base'!$C$40</f>
         <v>Semi-Automatic Scaling</v>
@@ -14530,12 +14506,12 @@
       <c r="AQ48" s="11"/>
       <c r="AR48" s="11"/>
       <c r="AS48" s="12"/>
-      <c r="AT48" s="142"/>
-      <c r="AU48" s="143"/>
-      <c r="AV48" s="143"/>
-      <c r="AW48" s="143"/>
-      <c r="AX48" s="143"/>
-      <c r="AY48" s="144"/>
+      <c r="AT48" s="144"/>
+      <c r="AU48" s="145"/>
+      <c r="AV48" s="145"/>
+      <c r="AW48" s="145"/>
+      <c r="AX48" s="145"/>
+      <c r="AY48" s="146"/>
       <c r="AZ48" s="11"/>
       <c r="BA48" s="11" t="s">
         <v>87</v>
@@ -14607,7 +14583,7 @@
       <c r="CT48" s="5"/>
     </row>
     <row r="49" spans="1:98" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="150"/>
+      <c r="A49" s="161"/>
       <c r="B49" s="113" t="str">
         <f>'Knowledge Base'!$C$41</f>
         <v>Semi-Automatic Third-Party Scaling</v>
@@ -14671,12 +14647,12 @@
       <c r="AQ49" s="11"/>
       <c r="AR49" s="11"/>
       <c r="AS49" s="12"/>
-      <c r="AT49" s="142"/>
-      <c r="AU49" s="143"/>
-      <c r="AV49" s="143"/>
-      <c r="AW49" s="143"/>
-      <c r="AX49" s="143"/>
-      <c r="AY49" s="144"/>
+      <c r="AT49" s="144"/>
+      <c r="AU49" s="145"/>
+      <c r="AV49" s="145"/>
+      <c r="AW49" s="145"/>
+      <c r="AX49" s="145"/>
+      <c r="AY49" s="146"/>
       <c r="AZ49" s="11"/>
       <c r="BA49" s="11" t="s">
         <v>87</v>
@@ -14748,7 +14724,7 @@
       <c r="CT49" s="5"/>
     </row>
     <row r="50" spans="1:98" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="150"/>
+      <c r="A50" s="161"/>
       <c r="B50" s="113" t="str">
         <f>'Knowledge Base'!$C$42</f>
         <v>Automatic Scaling</v>
@@ -14812,12 +14788,12 @@
       <c r="AQ50" s="11"/>
       <c r="AR50" s="11"/>
       <c r="AS50" s="12"/>
-      <c r="AT50" s="142"/>
-      <c r="AU50" s="143"/>
-      <c r="AV50" s="143"/>
-      <c r="AW50" s="143"/>
-      <c r="AX50" s="143"/>
-      <c r="AY50" s="144"/>
+      <c r="AT50" s="144"/>
+      <c r="AU50" s="145"/>
+      <c r="AV50" s="145"/>
+      <c r="AW50" s="145"/>
+      <c r="AX50" s="145"/>
+      <c r="AY50" s="146"/>
       <c r="AZ50" s="11"/>
       <c r="BA50" s="11" t="s">
         <v>87</v>
@@ -14889,7 +14865,7 @@
       <c r="CT50" s="5"/>
     </row>
     <row r="51" spans="1:98" s="19" customFormat="1" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="151"/>
+      <c r="A51" s="148"/>
       <c r="B51" s="115" t="str">
         <f>'Knowledge Base'!$C$43</f>
         <v>Automatic Third-Party Scaling</v>
@@ -14953,12 +14929,12 @@
       <c r="AQ51" s="35"/>
       <c r="AR51" s="35"/>
       <c r="AS51" s="36"/>
-      <c r="AT51" s="145"/>
-      <c r="AU51" s="146"/>
-      <c r="AV51" s="146"/>
-      <c r="AW51" s="146"/>
-      <c r="AX51" s="146"/>
-      <c r="AY51" s="147"/>
+      <c r="AT51" s="141"/>
+      <c r="AU51" s="147"/>
+      <c r="AV51" s="147"/>
+      <c r="AW51" s="147"/>
+      <c r="AX51" s="147"/>
+      <c r="AY51" s="142"/>
       <c r="AZ51" s="11"/>
       <c r="BA51" s="35" t="s">
         <v>87</v>
@@ -15100,12 +15076,12 @@
       <c r="AW52" s="137"/>
       <c r="AX52" s="137"/>
       <c r="AY52" s="138"/>
-      <c r="AZ52" s="142" t="s">
+      <c r="AZ52" s="144" t="s">
         <v>41</v>
       </c>
-      <c r="BA52" s="143"/>
-      <c r="BB52" s="143"/>
-      <c r="BC52" s="144"/>
+      <c r="BA52" s="145"/>
+      <c r="BB52" s="145"/>
+      <c r="BC52" s="146"/>
       <c r="BD52" s="11"/>
       <c r="BE52" s="137" t="str">
         <f>'Decision Level'!K10</f>
@@ -15175,7 +15151,7 @@
       <c r="CT52" s="5"/>
     </row>
     <row r="53" spans="1:98" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="150" t="str">
+      <c r="A53" s="161" t="str">
         <f>'Knowledge Base'!$B$44</f>
         <v>Select Scaling Trigger</v>
       </c>
@@ -15258,10 +15234,10 @@
       <c r="AY53" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AZ53" s="142"/>
-      <c r="BA53" s="143"/>
-      <c r="BB53" s="143"/>
-      <c r="BC53" s="144"/>
+      <c r="AZ53" s="144"/>
+      <c r="BA53" s="145"/>
+      <c r="BB53" s="145"/>
+      <c r="BC53" s="146"/>
       <c r="BD53" s="11"/>
       <c r="BE53" s="11"/>
       <c r="BF53" s="11"/>
@@ -15323,7 +15299,7 @@
       <c r="CT53" s="5"/>
     </row>
     <row r="54" spans="1:98" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="150"/>
+      <c r="A54" s="161"/>
       <c r="B54" s="113" t="str">
         <f>'Knowledge Base'!$C$45</f>
         <v>Event-Driven Trigger</v>
@@ -15403,10 +15379,10 @@
       <c r="AY54" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AZ54" s="142"/>
-      <c r="BA54" s="143"/>
-      <c r="BB54" s="143"/>
-      <c r="BC54" s="144"/>
+      <c r="AZ54" s="144"/>
+      <c r="BA54" s="145"/>
+      <c r="BB54" s="145"/>
+      <c r="BC54" s="146"/>
       <c r="BD54" s="11"/>
       <c r="BE54" s="11"/>
       <c r="BF54" s="11"/>
@@ -15468,7 +15444,7 @@
       <c r="CT54" s="5"/>
     </row>
     <row r="55" spans="1:98" s="19" customFormat="1" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="151"/>
+      <c r="A55" s="148"/>
       <c r="B55" s="115" t="str">
         <f>'Knowledge Base'!$C$46</f>
         <v>Proactive Trigger</v>
@@ -15548,10 +15524,10 @@
       <c r="AY55" s="36" t="s">
         <v>87</v>
       </c>
-      <c r="AZ55" s="145"/>
-      <c r="BA55" s="146"/>
-      <c r="BB55" s="146"/>
-      <c r="BC55" s="147"/>
+      <c r="AZ55" s="141"/>
+      <c r="BA55" s="147"/>
+      <c r="BB55" s="147"/>
+      <c r="BC55" s="142"/>
       <c r="BD55" s="35"/>
       <c r="BE55" s="35"/>
       <c r="BF55" s="35"/>
@@ -15693,10 +15669,10 @@
       <c r="BD56" s="139" t="s">
         <v>41</v>
       </c>
-      <c r="BE56" s="140"/>
-      <c r="BF56" s="140"/>
-      <c r="BG56" s="140"/>
-      <c r="BH56" s="141"/>
+      <c r="BE56" s="143"/>
+      <c r="BF56" s="143"/>
+      <c r="BG56" s="143"/>
+      <c r="BH56" s="140"/>
       <c r="BI56" s="11"/>
       <c r="BJ56" s="137" t="str">
         <f>'Decision Level'!L11</f>
@@ -15758,7 +15734,7 @@
       <c r="CT56" s="5"/>
     </row>
     <row r="57" spans="1:98" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="150" t="str">
+      <c r="A57" s="161" t="str">
         <f>'Knowledge Base'!$B$47</f>
         <v>Select Multi-Tenancy Level</v>
       </c>
@@ -15873,11 +15849,11 @@
       <c r="BA57" s="11"/>
       <c r="BB57" s="11"/>
       <c r="BC57" s="12"/>
-      <c r="BD57" s="142"/>
-      <c r="BE57" s="143"/>
-      <c r="BF57" s="143"/>
-      <c r="BG57" s="143"/>
-      <c r="BH57" s="144"/>
+      <c r="BD57" s="144"/>
+      <c r="BE57" s="145"/>
+      <c r="BF57" s="145"/>
+      <c r="BG57" s="145"/>
+      <c r="BH57" s="146"/>
       <c r="BI57" s="11"/>
       <c r="BJ57" s="59"/>
       <c r="BK57" s="11"/>
@@ -15934,7 +15910,7 @@
       <c r="CT57" s="5"/>
     </row>
     <row r="58" spans="1:98" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="150"/>
+      <c r="A58" s="161"/>
       <c r="B58" s="113" t="str">
         <f>'Knowledge Base'!$C$48</f>
         <v>Shared OS Multi-Tenancy</v>
@@ -16046,11 +16022,11 @@
       <c r="BA58" s="11"/>
       <c r="BB58" s="11"/>
       <c r="BC58" s="12"/>
-      <c r="BD58" s="142"/>
-      <c r="BE58" s="143"/>
-      <c r="BF58" s="143"/>
-      <c r="BG58" s="143"/>
-      <c r="BH58" s="144"/>
+      <c r="BD58" s="144"/>
+      <c r="BE58" s="145"/>
+      <c r="BF58" s="145"/>
+      <c r="BG58" s="145"/>
+      <c r="BH58" s="146"/>
       <c r="BI58" s="11"/>
       <c r="BJ58" s="59"/>
       <c r="BK58" s="11"/>
@@ -16107,7 +16083,7 @@
       <c r="CT58" s="5"/>
     </row>
     <row r="59" spans="1:98" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="150"/>
+      <c r="A59" s="161"/>
       <c r="B59" s="113" t="str">
         <f>'Knowledge Base'!$C$49</f>
         <v>Shared Middleware Multi-Tenancy</v>
@@ -16219,11 +16195,11 @@
       <c r="BA59" s="11"/>
       <c r="BB59" s="11"/>
       <c r="BC59" s="12"/>
-      <c r="BD59" s="142"/>
-      <c r="BE59" s="143"/>
-      <c r="BF59" s="143"/>
-      <c r="BG59" s="143"/>
-      <c r="BH59" s="144"/>
+      <c r="BD59" s="144"/>
+      <c r="BE59" s="145"/>
+      <c r="BF59" s="145"/>
+      <c r="BG59" s="145"/>
+      <c r="BH59" s="146"/>
       <c r="BI59" s="11"/>
       <c r="BJ59" s="11"/>
       <c r="BK59" s="11"/>
@@ -16280,7 +16256,7 @@
       <c r="CT59" s="5"/>
     </row>
     <row r="60" spans="1:98" s="19" customFormat="1" ht="15" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="151"/>
+      <c r="A60" s="148"/>
       <c r="B60" s="115" t="str">
         <f>'Knowledge Base'!$C$50</f>
         <v>Shared Application Multi-Tenancy</v>
@@ -16392,11 +16368,11 @@
       <c r="BA60" s="35"/>
       <c r="BB60" s="35"/>
       <c r="BC60" s="36"/>
-      <c r="BD60" s="145"/>
-      <c r="BE60" s="146"/>
-      <c r="BF60" s="146"/>
-      <c r="BG60" s="146"/>
-      <c r="BH60" s="147"/>
+      <c r="BD60" s="141"/>
+      <c r="BE60" s="147"/>
+      <c r="BF60" s="147"/>
+      <c r="BG60" s="147"/>
+      <c r="BH60" s="142"/>
       <c r="BI60" s="35"/>
       <c r="BJ60" s="35"/>
       <c r="BK60" s="35"/>
@@ -16541,10 +16517,10 @@
       <c r="BI61" s="139" t="s">
         <v>41</v>
       </c>
-      <c r="BJ61" s="140"/>
-      <c r="BK61" s="140"/>
-      <c r="BL61" s="140"/>
-      <c r="BM61" s="141"/>
+      <c r="BJ61" s="143"/>
+      <c r="BK61" s="143"/>
+      <c r="BL61" s="143"/>
+      <c r="BM61" s="140"/>
       <c r="BN61" s="11"/>
       <c r="BO61" s="137" t="str">
         <f>'Decision Level'!M12</f>
@@ -16598,7 +16574,7 @@
       <c r="CT61" s="5"/>
     </row>
     <row r="62" spans="1:98" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="150" t="str">
+      <c r="A62" s="161" t="str">
         <f>'Knowledge Base'!$B$51</f>
         <v>Select Cloud Deployment Model</v>
       </c>
@@ -16664,11 +16640,11 @@
       <c r="BF62" s="11"/>
       <c r="BG62" s="11"/>
       <c r="BH62" s="12"/>
-      <c r="BI62" s="142"/>
-      <c r="BJ62" s="143"/>
-      <c r="BK62" s="143"/>
-      <c r="BL62" s="143"/>
-      <c r="BM62" s="144"/>
+      <c r="BI62" s="144"/>
+      <c r="BJ62" s="145"/>
+      <c r="BK62" s="145"/>
+      <c r="BL62" s="145"/>
+      <c r="BM62" s="146"/>
       <c r="BN62" s="11"/>
       <c r="BO62" s="59"/>
       <c r="BP62" s="11"/>
@@ -16726,7 +16702,7 @@
       <c r="CT62" s="5"/>
     </row>
     <row r="63" spans="1:98" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="150"/>
+      <c r="A63" s="161"/>
       <c r="B63" s="113" t="str">
         <f>'Knowledge Base'!$C$52</f>
         <v>Private Cloud</v>
@@ -16789,11 +16765,11 @@
       <c r="BF63" s="11"/>
       <c r="BG63" s="11"/>
       <c r="BH63" s="12"/>
-      <c r="BI63" s="142"/>
-      <c r="BJ63" s="143"/>
-      <c r="BK63" s="143"/>
-      <c r="BL63" s="143"/>
-      <c r="BM63" s="144"/>
+      <c r="BI63" s="144"/>
+      <c r="BJ63" s="145"/>
+      <c r="BK63" s="145"/>
+      <c r="BL63" s="145"/>
+      <c r="BM63" s="146"/>
       <c r="BN63" s="11"/>
       <c r="BO63" s="59"/>
       <c r="BP63" s="11"/>
@@ -16851,7 +16827,7 @@
       <c r="CT63" s="5"/>
     </row>
     <row r="64" spans="1:98" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="150"/>
+      <c r="A64" s="161"/>
       <c r="B64" s="113" t="str">
         <f>'Knowledge Base'!$C$53</f>
         <v>Community Cloud</v>
@@ -16914,11 +16890,11 @@
       <c r="BF64" s="11"/>
       <c r="BG64" s="11"/>
       <c r="BH64" s="12"/>
-      <c r="BI64" s="142"/>
-      <c r="BJ64" s="143"/>
-      <c r="BK64" s="143"/>
-      <c r="BL64" s="143"/>
-      <c r="BM64" s="144"/>
+      <c r="BI64" s="144"/>
+      <c r="BJ64" s="145"/>
+      <c r="BK64" s="145"/>
+      <c r="BL64" s="145"/>
+      <c r="BM64" s="146"/>
       <c r="BN64" s="11"/>
       <c r="BO64" s="11"/>
       <c r="BP64" s="11"/>
@@ -16976,7 +16952,7 @@
       <c r="CT64" s="5"/>
     </row>
     <row r="65" spans="1:98" s="19" customFormat="1" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="151"/>
+      <c r="A65" s="148"/>
       <c r="B65" s="115" t="str">
         <f>'Knowledge Base'!$C$54</f>
         <v xml:space="preserve">Hybrid Cloud </v>
@@ -17039,11 +17015,11 @@
       <c r="BF65" s="35"/>
       <c r="BG65" s="35"/>
       <c r="BH65" s="36"/>
-      <c r="BI65" s="145"/>
-      <c r="BJ65" s="146"/>
-      <c r="BK65" s="146"/>
-      <c r="BL65" s="146"/>
-      <c r="BM65" s="147"/>
+      <c r="BI65" s="141"/>
+      <c r="BJ65" s="147"/>
+      <c r="BK65" s="147"/>
+      <c r="BL65" s="147"/>
+      <c r="BM65" s="142"/>
       <c r="BN65" s="35"/>
       <c r="BO65" s="35"/>
       <c r="BP65" s="35"/>
@@ -17197,13 +17173,13 @@
       <c r="BN66" s="139" t="s">
         <v>41</v>
       </c>
-      <c r="BO66" s="140"/>
-      <c r="BP66" s="140"/>
-      <c r="BQ66" s="140"/>
-      <c r="BR66" s="140"/>
-      <c r="BS66" s="140"/>
-      <c r="BT66" s="140"/>
-      <c r="BU66" s="141"/>
+      <c r="BO66" s="143"/>
+      <c r="BP66" s="143"/>
+      <c r="BQ66" s="143"/>
+      <c r="BR66" s="143"/>
+      <c r="BS66" s="143"/>
+      <c r="BT66" s="143"/>
+      <c r="BU66" s="140"/>
       <c r="BV66" s="11"/>
       <c r="BW66" s="137" t="str">
         <f>'Decision Level'!N13</f>
@@ -17246,7 +17222,7 @@
       <c r="CT66" s="5"/>
     </row>
     <row r="67" spans="1:98" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="150" t="str">
+      <c r="A67" s="161" t="str">
         <f>'Knowledge Base'!$B$55</f>
         <v>Select Cloud Service Model</v>
       </c>
@@ -17387,14 +17363,14 @@
       <c r="BK67" s="11"/>
       <c r="BL67" s="11"/>
       <c r="BM67" s="12"/>
-      <c r="BN67" s="142"/>
-      <c r="BO67" s="143"/>
-      <c r="BP67" s="143"/>
-      <c r="BQ67" s="143"/>
-      <c r="BR67" s="143"/>
-      <c r="BS67" s="143"/>
-      <c r="BT67" s="143"/>
-      <c r="BU67" s="144"/>
+      <c r="BN67" s="144"/>
+      <c r="BO67" s="145"/>
+      <c r="BP67" s="145"/>
+      <c r="BQ67" s="145"/>
+      <c r="BR67" s="145"/>
+      <c r="BS67" s="145"/>
+      <c r="BT67" s="145"/>
+      <c r="BU67" s="146"/>
       <c r="BV67" s="11"/>
       <c r="BW67" s="59"/>
       <c r="BX67" s="11"/>
@@ -17424,7 +17400,7 @@
       <c r="CT67" s="5"/>
     </row>
     <row r="68" spans="1:98" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="150"/>
+      <c r="A68" s="161"/>
       <c r="B68" s="113" t="str">
         <f>'Knowledge Base'!$C$56</f>
         <v xml:space="preserve">PaaS </v>
@@ -17561,14 +17537,14 @@
       <c r="BK68" s="11"/>
       <c r="BL68" s="11"/>
       <c r="BM68" s="12"/>
-      <c r="BN68" s="142"/>
-      <c r="BO68" s="143"/>
-      <c r="BP68" s="143"/>
-      <c r="BQ68" s="143"/>
-      <c r="BR68" s="143"/>
-      <c r="BS68" s="143"/>
-      <c r="BT68" s="143"/>
-      <c r="BU68" s="144"/>
+      <c r="BN68" s="144"/>
+      <c r="BO68" s="145"/>
+      <c r="BP68" s="145"/>
+      <c r="BQ68" s="145"/>
+      <c r="BR68" s="145"/>
+      <c r="BS68" s="145"/>
+      <c r="BT68" s="145"/>
+      <c r="BU68" s="146"/>
       <c r="BV68" s="11"/>
       <c r="BW68" s="11"/>
       <c r="BX68" s="11"/>
@@ -17598,7 +17574,7 @@
       <c r="CT68" s="5"/>
     </row>
     <row r="69" spans="1:98" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="150"/>
+      <c r="A69" s="161"/>
       <c r="B69" s="113" t="str">
         <f>'Knowledge Base'!$C$57</f>
         <v>SaaS</v>
@@ -17736,14 +17712,14 @@
       <c r="BK69" s="11"/>
       <c r="BL69" s="11"/>
       <c r="BM69" s="12"/>
-      <c r="BN69" s="142"/>
-      <c r="BO69" s="143"/>
-      <c r="BP69" s="143"/>
-      <c r="BQ69" s="143"/>
-      <c r="BR69" s="143"/>
-      <c r="BS69" s="143"/>
-      <c r="BT69" s="143"/>
-      <c r="BU69" s="144"/>
+      <c r="BN69" s="144"/>
+      <c r="BO69" s="145"/>
+      <c r="BP69" s="145"/>
+      <c r="BQ69" s="145"/>
+      <c r="BR69" s="145"/>
+      <c r="BS69" s="145"/>
+      <c r="BT69" s="145"/>
+      <c r="BU69" s="146"/>
       <c r="BV69" s="11"/>
       <c r="BW69" s="11"/>
       <c r="BX69" s="11"/>
@@ -17773,7 +17749,7 @@
       <c r="CT69" s="5"/>
     </row>
     <row r="70" spans="1:98" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="150"/>
+      <c r="A70" s="161"/>
       <c r="B70" s="113" t="str">
         <f>'Knowledge Base'!$C$58</f>
         <v>IaaS + PaaS</v>
@@ -17911,14 +17887,14 @@
       <c r="BK70" s="11"/>
       <c r="BL70" s="11"/>
       <c r="BM70" s="12"/>
-      <c r="BN70" s="142"/>
-      <c r="BO70" s="143"/>
-      <c r="BP70" s="143"/>
-      <c r="BQ70" s="143"/>
-      <c r="BR70" s="143"/>
-      <c r="BS70" s="143"/>
-      <c r="BT70" s="143"/>
-      <c r="BU70" s="144"/>
+      <c r="BN70" s="144"/>
+      <c r="BO70" s="145"/>
+      <c r="BP70" s="145"/>
+      <c r="BQ70" s="145"/>
+      <c r="BR70" s="145"/>
+      <c r="BS70" s="145"/>
+      <c r="BT70" s="145"/>
+      <c r="BU70" s="146"/>
       <c r="BV70" s="11"/>
       <c r="BW70" s="11"/>
       <c r="BX70" s="11"/>
@@ -17948,7 +17924,7 @@
       <c r="CT70" s="5"/>
     </row>
     <row r="71" spans="1:98" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="150"/>
+      <c r="A71" s="161"/>
       <c r="B71" s="113" t="str">
         <f>'Knowledge Base'!$C$59</f>
         <v>IaaS + SaaS</v>
@@ -18086,14 +18062,14 @@
       <c r="BK71" s="11"/>
       <c r="BL71" s="11"/>
       <c r="BM71" s="12"/>
-      <c r="BN71" s="142"/>
-      <c r="BO71" s="143"/>
-      <c r="BP71" s="143"/>
-      <c r="BQ71" s="143"/>
-      <c r="BR71" s="143"/>
-      <c r="BS71" s="143"/>
-      <c r="BT71" s="143"/>
-      <c r="BU71" s="144"/>
+      <c r="BN71" s="144"/>
+      <c r="BO71" s="145"/>
+      <c r="BP71" s="145"/>
+      <c r="BQ71" s="145"/>
+      <c r="BR71" s="145"/>
+      <c r="BS71" s="145"/>
+      <c r="BT71" s="145"/>
+      <c r="BU71" s="146"/>
       <c r="BV71" s="11"/>
       <c r="BW71" s="11"/>
       <c r="BX71" s="11"/>
@@ -18123,7 +18099,7 @@
       <c r="CT71" s="5"/>
     </row>
     <row r="72" spans="1:98" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="150"/>
+      <c r="A72" s="161"/>
       <c r="B72" s="113" t="str">
         <f>'Knowledge Base'!$C$60</f>
         <v>PaaS + SaaS</v>
@@ -18261,14 +18237,14 @@
       <c r="BK72" s="11"/>
       <c r="BL72" s="11"/>
       <c r="BM72" s="12"/>
-      <c r="BN72" s="142"/>
-      <c r="BO72" s="143"/>
-      <c r="BP72" s="143"/>
-      <c r="BQ72" s="143"/>
-      <c r="BR72" s="143"/>
-      <c r="BS72" s="143"/>
-      <c r="BT72" s="143"/>
-      <c r="BU72" s="144"/>
+      <c r="BN72" s="144"/>
+      <c r="BO72" s="145"/>
+      <c r="BP72" s="145"/>
+      <c r="BQ72" s="145"/>
+      <c r="BR72" s="145"/>
+      <c r="BS72" s="145"/>
+      <c r="BT72" s="145"/>
+      <c r="BU72" s="146"/>
       <c r="BV72" s="11"/>
       <c r="BW72" s="11"/>
       <c r="BX72" s="11"/>
@@ -18298,7 +18274,7 @@
       <c r="CT72" s="5"/>
     </row>
     <row r="73" spans="1:98" s="19" customFormat="1" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="151"/>
+      <c r="A73" s="148"/>
       <c r="B73" s="115" t="str">
         <f>'Knowledge Base'!$C$61</f>
         <v>Iaas + PaaS + SaaS</v>
@@ -18436,14 +18412,14 @@
       <c r="BK73" s="35"/>
       <c r="BL73" s="35"/>
       <c r="BM73" s="36"/>
-      <c r="BN73" s="145"/>
-      <c r="BO73" s="146"/>
-      <c r="BP73" s="146"/>
-      <c r="BQ73" s="146"/>
-      <c r="BR73" s="146"/>
-      <c r="BS73" s="146"/>
-      <c r="BT73" s="146"/>
-      <c r="BU73" s="147"/>
+      <c r="BN73" s="141"/>
+      <c r="BO73" s="147"/>
+      <c r="BP73" s="147"/>
+      <c r="BQ73" s="147"/>
+      <c r="BR73" s="147"/>
+      <c r="BS73" s="147"/>
+      <c r="BT73" s="147"/>
+      <c r="BU73" s="142"/>
       <c r="BV73" s="35"/>
       <c r="BW73" s="35"/>
       <c r="BX73" s="35"/>
@@ -18580,8 +18556,8 @@
       <c r="BV74" s="139" t="s">
         <v>41</v>
       </c>
-      <c r="BW74" s="140"/>
-      <c r="BX74" s="140"/>
+      <c r="BW74" s="143"/>
+      <c r="BX74" s="143"/>
       <c r="BY74" s="124"/>
       <c r="BZ74" s="11"/>
       <c r="CA74" s="137" t="str">
@@ -18618,7 +18594,7 @@
       <c r="CT74" s="5"/>
     </row>
     <row r="75" spans="1:98" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="150" t="str">
+      <c r="A75" s="161" t="str">
         <f>'Knowledge Base'!$B$62</f>
         <v>Define Cloud Hosting</v>
       </c>
@@ -18705,9 +18681,9 @@
       <c r="BS75" s="11"/>
       <c r="BT75" s="11"/>
       <c r="BU75" s="12"/>
-      <c r="BV75" s="142"/>
-      <c r="BW75" s="143"/>
-      <c r="BX75" s="143"/>
+      <c r="BV75" s="144"/>
+      <c r="BW75" s="145"/>
+      <c r="BX75" s="145"/>
       <c r="BY75" s="124"/>
       <c r="BZ75" s="11"/>
       <c r="CA75" s="59" t="s">
@@ -18752,7 +18728,7 @@
       <c r="CT75" s="5"/>
     </row>
     <row r="76" spans="1:98" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="150"/>
+      <c r="A76" s="161"/>
       <c r="B76" s="113" t="str">
         <f>'Knowledge Base'!$C$63</f>
         <v>Off-Premise Hosting</v>
@@ -18836,9 +18812,9 @@
       <c r="BS76" s="11"/>
       <c r="BT76" s="11"/>
       <c r="BU76" s="12"/>
-      <c r="BV76" s="142"/>
-      <c r="BW76" s="143"/>
-      <c r="BX76" s="143"/>
+      <c r="BV76" s="144"/>
+      <c r="BW76" s="145"/>
+      <c r="BX76" s="145"/>
       <c r="BY76" s="124"/>
       <c r="BZ76" s="11"/>
       <c r="CA76" s="59" t="s">
@@ -18883,7 +18859,7 @@
       <c r="CT76" s="5"/>
     </row>
     <row r="77" spans="1:98" s="19" customFormat="1" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="151"/>
+      <c r="A77" s="148"/>
       <c r="B77" s="115" t="str">
         <f>'Knowledge Base'!$C$64</f>
         <v>Hybrid Hosting</v>
@@ -18967,9 +18943,9 @@
       <c r="BS77" s="35"/>
       <c r="BT77" s="35"/>
       <c r="BU77" s="36"/>
-      <c r="BV77" s="145"/>
-      <c r="BW77" s="146"/>
-      <c r="BX77" s="146"/>
+      <c r="BV77" s="141"/>
+      <c r="BW77" s="147"/>
+      <c r="BX77" s="147"/>
       <c r="BY77" s="125"/>
       <c r="BZ77" s="35"/>
       <c r="CA77" s="61" t="s">
@@ -19128,13 +19104,13 @@
       <c r="BZ78" s="139" t="s">
         <v>41</v>
       </c>
-      <c r="CA78" s="140"/>
-      <c r="CB78" s="140"/>
-      <c r="CC78" s="140"/>
-      <c r="CD78" s="140"/>
-      <c r="CE78" s="140"/>
-      <c r="CF78" s="140"/>
-      <c r="CG78" s="141"/>
+      <c r="CA78" s="143"/>
+      <c r="CB78" s="143"/>
+      <c r="CC78" s="143"/>
+      <c r="CD78" s="143"/>
+      <c r="CE78" s="143"/>
+      <c r="CF78" s="143"/>
+      <c r="CG78" s="140"/>
       <c r="CH78" s="11"/>
       <c r="CI78" s="14" t="str">
         <f>'Decision Level'!P15</f>
@@ -19159,7 +19135,7 @@
       <c r="CT78" s="5"/>
     </row>
     <row r="79" spans="1:98" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="150" t="str">
+      <c r="A79" s="161" t="str">
         <f>'Knowledge Base'!$B$65</f>
         <v>Define Roles of Responsibility</v>
       </c>
@@ -19256,14 +19232,14 @@
       <c r="BY79" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="BZ79" s="142"/>
-      <c r="CA79" s="143"/>
-      <c r="CB79" s="143"/>
-      <c r="CC79" s="143"/>
-      <c r="CD79" s="143"/>
-      <c r="CE79" s="143"/>
-      <c r="CF79" s="143"/>
-      <c r="CG79" s="144"/>
+      <c r="BZ79" s="144"/>
+      <c r="CA79" s="145"/>
+      <c r="CB79" s="145"/>
+      <c r="CC79" s="145"/>
+      <c r="CD79" s="145"/>
+      <c r="CE79" s="145"/>
+      <c r="CF79" s="145"/>
+      <c r="CG79" s="146"/>
       <c r="CH79" s="11"/>
       <c r="CI79" s="60" t="s">
         <v>106</v>
@@ -19281,7 +19257,7 @@
       <c r="CT79" s="5"/>
     </row>
     <row r="80" spans="1:98" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="150"/>
+      <c r="A80" s="161"/>
       <c r="B80" s="113" t="str">
         <f>'Knowledge Base'!$C$66</f>
         <v>Managmenet</v>
@@ -19375,14 +19351,14 @@
       <c r="BY80" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="BZ80" s="142"/>
-      <c r="CA80" s="143"/>
-      <c r="CB80" s="143"/>
-      <c r="CC80" s="143"/>
-      <c r="CD80" s="143"/>
-      <c r="CE80" s="143"/>
-      <c r="CF80" s="143"/>
-      <c r="CG80" s="144"/>
+      <c r="BZ80" s="144"/>
+      <c r="CA80" s="145"/>
+      <c r="CB80" s="145"/>
+      <c r="CC80" s="145"/>
+      <c r="CD80" s="145"/>
+      <c r="CE80" s="145"/>
+      <c r="CF80" s="145"/>
+      <c r="CG80" s="146"/>
       <c r="CH80" s="11"/>
       <c r="CI80" s="60" t="s">
         <v>106</v>
@@ -19400,7 +19376,7 @@
       <c r="CT80" s="5"/>
     </row>
     <row r="81" spans="1:98" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="150"/>
+      <c r="A81" s="161"/>
       <c r="B81" s="113" t="str">
         <f>'Knowledge Base'!$C$67</f>
         <v>Outsourced</v>
@@ -19494,14 +19470,14 @@
       <c r="BY81" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="BZ81" s="142"/>
-      <c r="CA81" s="143"/>
-      <c r="CB81" s="143"/>
-      <c r="CC81" s="143"/>
-      <c r="CD81" s="143"/>
-      <c r="CE81" s="143"/>
-      <c r="CF81" s="143"/>
-      <c r="CG81" s="144"/>
+      <c r="BZ81" s="144"/>
+      <c r="CA81" s="145"/>
+      <c r="CB81" s="145"/>
+      <c r="CC81" s="145"/>
+      <c r="CD81" s="145"/>
+      <c r="CE81" s="145"/>
+      <c r="CF81" s="145"/>
+      <c r="CG81" s="146"/>
       <c r="CH81" s="11"/>
       <c r="CI81" s="60" t="s">
         <v>106</v>
@@ -19519,7 +19495,7 @@
       <c r="CT81" s="5"/>
     </row>
     <row r="82" spans="1:98" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="150"/>
+      <c r="A82" s="161"/>
       <c r="B82" s="113" t="str">
         <f>'Knowledge Base'!$C$68</f>
         <v>Inhouse + Management</v>
@@ -19612,14 +19588,14 @@
       <c r="BY82" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="BZ82" s="142"/>
-      <c r="CA82" s="143"/>
-      <c r="CB82" s="143"/>
-      <c r="CC82" s="143"/>
-      <c r="CD82" s="143"/>
-      <c r="CE82" s="143"/>
-      <c r="CF82" s="143"/>
-      <c r="CG82" s="144"/>
+      <c r="BZ82" s="144"/>
+      <c r="CA82" s="145"/>
+      <c r="CB82" s="145"/>
+      <c r="CC82" s="145"/>
+      <c r="CD82" s="145"/>
+      <c r="CE82" s="145"/>
+      <c r="CF82" s="145"/>
+      <c r="CG82" s="146"/>
       <c r="CH82" s="11"/>
       <c r="CI82" s="12" t="s">
         <v>106</v>
@@ -19637,7 +19613,7 @@
       <c r="CT82" s="5"/>
     </row>
     <row r="83" spans="1:98" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="150"/>
+      <c r="A83" s="161"/>
       <c r="B83" s="113" t="str">
         <f>'Knowledge Base'!$C$69</f>
         <v>Inhouse + Outsourced</v>
@@ -19731,14 +19707,14 @@
       <c r="BY83" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="BZ83" s="142"/>
-      <c r="CA83" s="143"/>
-      <c r="CB83" s="143"/>
-      <c r="CC83" s="143"/>
-      <c r="CD83" s="143"/>
-      <c r="CE83" s="143"/>
-      <c r="CF83" s="143"/>
-      <c r="CG83" s="144"/>
+      <c r="BZ83" s="144"/>
+      <c r="CA83" s="145"/>
+      <c r="CB83" s="145"/>
+      <c r="CC83" s="145"/>
+      <c r="CD83" s="145"/>
+      <c r="CE83" s="145"/>
+      <c r="CF83" s="145"/>
+      <c r="CG83" s="146"/>
       <c r="CH83" s="11"/>
       <c r="CI83" s="12" t="s">
         <v>106</v>
@@ -19756,7 +19732,7 @@
       <c r="CT83" s="5"/>
     </row>
     <row r="84" spans="1:98" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="150"/>
+      <c r="A84" s="161"/>
       <c r="B84" s="113" t="str">
         <f>'Knowledge Base'!$C$70</f>
         <v>Management + Outsourced</v>
@@ -19850,14 +19826,14 @@
       <c r="BY84" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="BZ84" s="142"/>
-      <c r="CA84" s="143"/>
-      <c r="CB84" s="143"/>
-      <c r="CC84" s="143"/>
-      <c r="CD84" s="143"/>
-      <c r="CE84" s="143"/>
-      <c r="CF84" s="143"/>
-      <c r="CG84" s="144"/>
+      <c r="BZ84" s="144"/>
+      <c r="CA84" s="145"/>
+      <c r="CB84" s="145"/>
+      <c r="CC84" s="145"/>
+      <c r="CD84" s="145"/>
+      <c r="CE84" s="145"/>
+      <c r="CF84" s="145"/>
+      <c r="CG84" s="146"/>
       <c r="CH84" s="11"/>
       <c r="CI84" s="12" t="s">
         <v>106</v>
@@ -19875,7 +19851,7 @@
       <c r="CT84" s="5"/>
     </row>
     <row r="85" spans="1:98" s="19" customFormat="1" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="151"/>
+      <c r="A85" s="148"/>
       <c r="B85" s="115" t="str">
         <f>'Knowledge Base'!$C$71</f>
         <v>Inhouse + Management + Outsourced</v>
@@ -19969,14 +19945,14 @@
       <c r="BY85" s="36" t="s">
         <v>85</v>
       </c>
-      <c r="BZ85" s="145"/>
-      <c r="CA85" s="146"/>
-      <c r="CB85" s="146"/>
-      <c r="CC85" s="146"/>
-      <c r="CD85" s="146"/>
-      <c r="CE85" s="146"/>
-      <c r="CF85" s="146"/>
-      <c r="CG85" s="147"/>
+      <c r="BZ85" s="141"/>
+      <c r="CA85" s="147"/>
+      <c r="CB85" s="147"/>
+      <c r="CC85" s="147"/>
+      <c r="CD85" s="147"/>
+      <c r="CE85" s="147"/>
+      <c r="CF85" s="147"/>
+      <c r="CG85" s="142"/>
       <c r="CH85" s="35"/>
       <c r="CI85" s="36" t="s">
         <v>106</v>
@@ -20121,7 +20097,7 @@
       <c r="CH86" s="139" t="s">
         <v>41</v>
       </c>
-      <c r="CI86" s="141"/>
+      <c r="CI86" s="140"/>
       <c r="CJ86" s="62"/>
       <c r="CK86" s="137" t="str">
         <f>'Decision Level'!Q16</f>
@@ -20320,8 +20296,8 @@
       <c r="CG87" s="36" t="s">
         <v>88</v>
       </c>
-      <c r="CH87" s="145"/>
-      <c r="CI87" s="147"/>
+      <c r="CH87" s="141"/>
+      <c r="CI87" s="142"/>
       <c r="CJ87" s="35"/>
       <c r="CK87" s="61" t="s">
         <v>88</v>
@@ -20477,10 +20453,10 @@
       <c r="CJ88" s="139" t="s">
         <v>41</v>
       </c>
-      <c r="CK88" s="140"/>
-      <c r="CL88" s="140"/>
-      <c r="CM88" s="140"/>
-      <c r="CN88" s="141"/>
+      <c r="CK88" s="143"/>
+      <c r="CL88" s="143"/>
+      <c r="CM88" s="143"/>
+      <c r="CN88" s="140"/>
       <c r="CO88" s="11"/>
       <c r="CP88" s="137" t="str">
         <f>'Decision Level'!R17</f>
@@ -20492,7 +20468,7 @@
       <c r="CT88" s="5"/>
     </row>
     <row r="89" spans="1:98" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="150" t="str">
+      <c r="A89" s="161" t="str">
         <f>'Knowledge Base'!$B$73</f>
         <v>Select Pricing Model</v>
       </c>
@@ -20587,11 +20563,11 @@
       <c r="CI89" s="60" t="s">
         <v>106</v>
       </c>
-      <c r="CJ89" s="142"/>
-      <c r="CK89" s="143"/>
-      <c r="CL89" s="143"/>
-      <c r="CM89" s="143"/>
-      <c r="CN89" s="144"/>
+      <c r="CJ89" s="144"/>
+      <c r="CK89" s="145"/>
+      <c r="CL89" s="145"/>
+      <c r="CM89" s="145"/>
+      <c r="CN89" s="146"/>
       <c r="CO89" s="11"/>
       <c r="CP89" s="59"/>
       <c r="CQ89" s="12"/>
@@ -20600,7 +20576,7 @@
       <c r="CT89" s="5"/>
     </row>
     <row r="90" spans="1:98" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="150"/>
+      <c r="A90" s="161"/>
       <c r="B90" s="113" t="str">
         <f>'Knowledge Base'!$C$74</f>
         <v>Pay-Per-Use</v>
@@ -20692,11 +20668,11 @@
       <c r="CI90" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="CJ90" s="142"/>
-      <c r="CK90" s="143"/>
-      <c r="CL90" s="143"/>
-      <c r="CM90" s="143"/>
-      <c r="CN90" s="144"/>
+      <c r="CJ90" s="144"/>
+      <c r="CK90" s="145"/>
+      <c r="CL90" s="145"/>
+      <c r="CM90" s="145"/>
+      <c r="CN90" s="146"/>
       <c r="CO90" s="11"/>
       <c r="CP90" s="11"/>
       <c r="CQ90" s="12"/>
@@ -20705,7 +20681,7 @@
       <c r="CT90" s="5"/>
     </row>
     <row r="91" spans="1:98" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="150"/>
+      <c r="A91" s="161"/>
       <c r="B91" s="113" t="str">
         <f>'Knowledge Base'!$C$75</f>
         <v>Pay-Per-Unit</v>
@@ -20797,11 +20773,11 @@
       <c r="CI91" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="CJ91" s="142"/>
-      <c r="CK91" s="143"/>
-      <c r="CL91" s="143"/>
-      <c r="CM91" s="143"/>
-      <c r="CN91" s="144"/>
+      <c r="CJ91" s="144"/>
+      <c r="CK91" s="145"/>
+      <c r="CL91" s="145"/>
+      <c r="CM91" s="145"/>
+      <c r="CN91" s="146"/>
       <c r="CO91" s="11"/>
       <c r="CP91" s="11"/>
       <c r="CQ91" s="12"/>
@@ -20810,7 +20786,7 @@
       <c r="CT91" s="5"/>
     </row>
     <row r="92" spans="1:98" s="19" customFormat="1" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="151"/>
+      <c r="A92" s="148"/>
       <c r="B92" s="115" t="str">
         <f>'Knowledge Base'!$C$76</f>
         <v>Charge-Per-Use (Subscription)</v>
@@ -20902,11 +20878,11 @@
       <c r="CI92" s="36" t="s">
         <v>106</v>
       </c>
-      <c r="CJ92" s="145"/>
-      <c r="CK92" s="146"/>
-      <c r="CL92" s="146"/>
-      <c r="CM92" s="146"/>
-      <c r="CN92" s="147"/>
+      <c r="CJ92" s="141"/>
+      <c r="CK92" s="147"/>
+      <c r="CL92" s="147"/>
+      <c r="CM92" s="147"/>
+      <c r="CN92" s="142"/>
       <c r="CO92" s="35"/>
       <c r="CP92" s="35"/>
       <c r="CQ92" s="36"/>
@@ -20916,16 +20892,16 @@
     </row>
     <row r="93" spans="1:98" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C93" s="11"/>
-      <c r="D93" s="148" t="str">
+      <c r="D93" s="162" t="str">
         <f>'Decision Level'!$C$18</f>
         <v>N/A</v>
       </c>
-      <c r="E93" s="148"/>
-      <c r="F93" s="148"/>
-      <c r="G93" s="148"/>
-      <c r="H93" s="148"/>
-      <c r="I93" s="148"/>
-      <c r="J93" s="149"/>
+      <c r="E93" s="162"/>
+      <c r="F93" s="162"/>
+      <c r="G93" s="162"/>
+      <c r="H93" s="162"/>
+      <c r="I93" s="162"/>
+      <c r="J93" s="163"/>
       <c r="K93" s="11"/>
       <c r="L93" s="137" t="str">
         <f>'Decision Level'!D18</f>
@@ -21053,14 +21029,14 @@
       <c r="CO93" s="139" t="s">
         <v>41</v>
       </c>
-      <c r="CP93" s="140"/>
-      <c r="CQ93" s="141"/>
+      <c r="CP93" s="143"/>
+      <c r="CQ93" s="140"/>
       <c r="CR93" s="5"/>
       <c r="CS93" s="5"/>
       <c r="CT93" s="5"/>
     </row>
     <row r="94" spans="1:98" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="150" t="str">
+      <c r="A94" s="161" t="str">
         <f>'Knowledge Base'!$B$77</f>
         <v>Define Resource Location</v>
       </c>
@@ -21166,15 +21142,15 @@
       <c r="CL94" s="11"/>
       <c r="CM94" s="11"/>
       <c r="CN94" s="12"/>
-      <c r="CO94" s="142"/>
-      <c r="CP94" s="143"/>
-      <c r="CQ94" s="144"/>
+      <c r="CO94" s="144"/>
+      <c r="CP94" s="145"/>
+      <c r="CQ94" s="146"/>
       <c r="CR94" s="5"/>
       <c r="CS94" s="5"/>
       <c r="CT94" s="5"/>
     </row>
     <row r="95" spans="1:98" s="19" customFormat="1" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A95" s="151"/>
+      <c r="A95" s="148"/>
       <c r="B95" s="115" t="str">
         <f>'Knowledge Base'!$C$78</f>
         <v>Data In Different Jurisdiction</v>
@@ -21277,9 +21253,9 @@
       <c r="CL95" s="35"/>
       <c r="CM95" s="35"/>
       <c r="CN95" s="36"/>
-      <c r="CO95" s="145"/>
-      <c r="CP95" s="146"/>
-      <c r="CQ95" s="147"/>
+      <c r="CO95" s="141"/>
+      <c r="CP95" s="147"/>
+      <c r="CQ95" s="142"/>
       <c r="CR95" s="39"/>
       <c r="CS95" s="39"/>
       <c r="CT95" s="39"/>
@@ -27459,25 +27435,234 @@
     </row>
   </sheetData>
   <mergeCells count="271">
-    <mergeCell ref="D61:J61"/>
-    <mergeCell ref="AQ61:AS61"/>
-    <mergeCell ref="AU61:AY61"/>
-    <mergeCell ref="BA61:BC61"/>
-    <mergeCell ref="BE61:BH61"/>
-    <mergeCell ref="BO61:BU61"/>
-    <mergeCell ref="AC61:AF61"/>
-    <mergeCell ref="AH61:AO61"/>
-    <mergeCell ref="L61:R61"/>
-    <mergeCell ref="T61:AA61"/>
-    <mergeCell ref="AQ56:AS56"/>
-    <mergeCell ref="AH56:AO56"/>
-    <mergeCell ref="AC56:AF56"/>
-    <mergeCell ref="CP56:CQ56"/>
-    <mergeCell ref="CK56:CN56"/>
-    <mergeCell ref="CA56:CG56"/>
-    <mergeCell ref="BW56:BY56"/>
-    <mergeCell ref="BO56:BU56"/>
-    <mergeCell ref="BJ56:BM56"/>
+    <mergeCell ref="BO86:BU86"/>
+    <mergeCell ref="BJ86:BM86"/>
+    <mergeCell ref="BE86:BH86"/>
+    <mergeCell ref="BA86:BC86"/>
+    <mergeCell ref="CA86:CG86"/>
+    <mergeCell ref="BW86:BY86"/>
+    <mergeCell ref="CP86:CQ86"/>
+    <mergeCell ref="CK86:CN86"/>
+    <mergeCell ref="CA33:CG33"/>
+    <mergeCell ref="BW33:BY33"/>
+    <mergeCell ref="CP33:CQ33"/>
+    <mergeCell ref="CK33:CN33"/>
+    <mergeCell ref="BE42:BH42"/>
+    <mergeCell ref="BA42:BC42"/>
+    <mergeCell ref="CP52:CQ52"/>
+    <mergeCell ref="CK52:CN52"/>
+    <mergeCell ref="CK66:CN66"/>
+    <mergeCell ref="CP66:CQ66"/>
+    <mergeCell ref="CA66:CG66"/>
+    <mergeCell ref="BJ66:BM66"/>
+    <mergeCell ref="BW66:BY66"/>
+    <mergeCell ref="BA66:BC66"/>
+    <mergeCell ref="BE66:BH66"/>
+    <mergeCell ref="BW78:BY78"/>
+    <mergeCell ref="L33:R33"/>
+    <mergeCell ref="D33:J33"/>
+    <mergeCell ref="AC33:AF33"/>
+    <mergeCell ref="T33:AA33"/>
+    <mergeCell ref="BA33:BC33"/>
+    <mergeCell ref="AU33:AY33"/>
+    <mergeCell ref="AQ33:AS33"/>
+    <mergeCell ref="BO33:BU33"/>
+    <mergeCell ref="BJ33:BM33"/>
+    <mergeCell ref="BE33:BH33"/>
+    <mergeCell ref="AU42:AY42"/>
+    <mergeCell ref="BO42:BU42"/>
+    <mergeCell ref="BJ42:BM42"/>
+    <mergeCell ref="CA42:CG42"/>
+    <mergeCell ref="BW42:BY42"/>
+    <mergeCell ref="CP42:CQ42"/>
+    <mergeCell ref="CK42:CN42"/>
+    <mergeCell ref="AH46:AO46"/>
+    <mergeCell ref="AQ46:AS46"/>
+    <mergeCell ref="CA46:CG46"/>
+    <mergeCell ref="CK46:CN46"/>
+    <mergeCell ref="CP46:CQ46"/>
+    <mergeCell ref="BJ46:BM46"/>
+    <mergeCell ref="BO46:BU46"/>
+    <mergeCell ref="BW46:BY46"/>
+    <mergeCell ref="BA46:BC46"/>
+    <mergeCell ref="BE46:BH46"/>
+    <mergeCell ref="AT46:AY51"/>
+    <mergeCell ref="D46:J46"/>
+    <mergeCell ref="L46:R46"/>
+    <mergeCell ref="T46:AA46"/>
+    <mergeCell ref="AC46:AF46"/>
+    <mergeCell ref="AH42:AO42"/>
+    <mergeCell ref="AC42:AF42"/>
+    <mergeCell ref="T42:AA42"/>
+    <mergeCell ref="L42:R42"/>
+    <mergeCell ref="D42:J42"/>
+    <mergeCell ref="AQ78:AS78"/>
+    <mergeCell ref="AC52:AF52"/>
+    <mergeCell ref="T52:AA52"/>
+    <mergeCell ref="L52:R52"/>
+    <mergeCell ref="D52:J52"/>
+    <mergeCell ref="AU52:AY52"/>
+    <mergeCell ref="AQ52:AS52"/>
+    <mergeCell ref="AH52:AO52"/>
+    <mergeCell ref="CA52:CG52"/>
+    <mergeCell ref="BW52:BY52"/>
+    <mergeCell ref="BO52:BU52"/>
+    <mergeCell ref="BJ52:BM52"/>
+    <mergeCell ref="BE52:BH52"/>
+    <mergeCell ref="AZ52:BC55"/>
+    <mergeCell ref="AU78:AY78"/>
+    <mergeCell ref="BA78:BC78"/>
+    <mergeCell ref="BE78:BH78"/>
+    <mergeCell ref="BJ78:BM78"/>
+    <mergeCell ref="T78:AA78"/>
+    <mergeCell ref="AC78:AF78"/>
+    <mergeCell ref="AH78:AO78"/>
+    <mergeCell ref="L66:R66"/>
+    <mergeCell ref="D66:J66"/>
+    <mergeCell ref="AC66:AF66"/>
+    <mergeCell ref="T88:AA88"/>
+    <mergeCell ref="L88:R88"/>
+    <mergeCell ref="D88:J88"/>
+    <mergeCell ref="AU86:AY86"/>
+    <mergeCell ref="AQ86:AS86"/>
+    <mergeCell ref="AH86:AO86"/>
+    <mergeCell ref="AC86:AF86"/>
+    <mergeCell ref="T86:AA86"/>
+    <mergeCell ref="L86:R86"/>
+    <mergeCell ref="D86:J86"/>
+    <mergeCell ref="D93:J93"/>
+    <mergeCell ref="BA93:BC93"/>
+    <mergeCell ref="AU93:AY93"/>
+    <mergeCell ref="AQ93:AS93"/>
+    <mergeCell ref="BO93:BU93"/>
+    <mergeCell ref="BJ93:BM93"/>
+    <mergeCell ref="BE93:BH93"/>
+    <mergeCell ref="T93:AA93"/>
+    <mergeCell ref="L93:R93"/>
+    <mergeCell ref="BJ88:BM88"/>
+    <mergeCell ref="CA88:CG88"/>
+    <mergeCell ref="BW88:BY88"/>
+    <mergeCell ref="CP88:CQ88"/>
+    <mergeCell ref="AH93:AO93"/>
+    <mergeCell ref="AC93:AF93"/>
+    <mergeCell ref="CK93:CN93"/>
+    <mergeCell ref="BE88:BH88"/>
+    <mergeCell ref="BA88:BC88"/>
+    <mergeCell ref="AU88:AY88"/>
+    <mergeCell ref="AQ88:AS88"/>
+    <mergeCell ref="AH88:AO88"/>
+    <mergeCell ref="AC88:AF88"/>
+    <mergeCell ref="T66:AA66"/>
+    <mergeCell ref="AC74:AF74"/>
+    <mergeCell ref="T74:AA74"/>
+    <mergeCell ref="L74:R74"/>
+    <mergeCell ref="D74:J74"/>
+    <mergeCell ref="AU74:AY74"/>
+    <mergeCell ref="AQ74:AS74"/>
+    <mergeCell ref="AH74:AO74"/>
+    <mergeCell ref="AH66:AO66"/>
+    <mergeCell ref="BA74:BC74"/>
+    <mergeCell ref="AQ66:AS66"/>
+    <mergeCell ref="AU66:AY66"/>
+    <mergeCell ref="D78:J78"/>
+    <mergeCell ref="L78:R78"/>
+    <mergeCell ref="BW28:BY28"/>
+    <mergeCell ref="CA28:CG28"/>
+    <mergeCell ref="CK28:CN28"/>
+    <mergeCell ref="CP28:CQ28"/>
+    <mergeCell ref="D28:J28"/>
+    <mergeCell ref="T28:AA28"/>
+    <mergeCell ref="L28:R28"/>
+    <mergeCell ref="BA28:BC28"/>
+    <mergeCell ref="AU28:AY28"/>
+    <mergeCell ref="AQ28:AS28"/>
+    <mergeCell ref="AH28:AO28"/>
+    <mergeCell ref="BO28:BU28"/>
+    <mergeCell ref="BJ28:BM28"/>
+    <mergeCell ref="BE28:BH28"/>
+    <mergeCell ref="T56:AA56"/>
+    <mergeCell ref="L56:R56"/>
+    <mergeCell ref="D56:J56"/>
+    <mergeCell ref="BA56:BC56"/>
+    <mergeCell ref="AU56:AY56"/>
+    <mergeCell ref="CA3:CG3"/>
+    <mergeCell ref="CK19:CN19"/>
+    <mergeCell ref="CP19:CQ19"/>
+    <mergeCell ref="BA19:BC19"/>
+    <mergeCell ref="BE19:BH19"/>
+    <mergeCell ref="BJ19:BM19"/>
+    <mergeCell ref="BO19:BU19"/>
+    <mergeCell ref="T11:AA11"/>
+    <mergeCell ref="L3:R3"/>
+    <mergeCell ref="BW19:BY19"/>
+    <mergeCell ref="CA19:CG19"/>
+    <mergeCell ref="L19:R19"/>
+    <mergeCell ref="AC19:AF19"/>
+    <mergeCell ref="AH19:AO19"/>
+    <mergeCell ref="AQ19:AS19"/>
+    <mergeCell ref="AU19:AY19"/>
+    <mergeCell ref="AQ11:AS11"/>
+    <mergeCell ref="AU11:AY11"/>
+    <mergeCell ref="BA11:BC11"/>
+    <mergeCell ref="BE11:BH11"/>
+    <mergeCell ref="AC11:AF11"/>
+    <mergeCell ref="AH11:AO11"/>
+    <mergeCell ref="CK3:CN3"/>
+    <mergeCell ref="A20:A27"/>
+    <mergeCell ref="A12:A18"/>
+    <mergeCell ref="A4:A10"/>
+    <mergeCell ref="BE2:BH2"/>
+    <mergeCell ref="BA2:BC2"/>
+    <mergeCell ref="AU2:AY2"/>
+    <mergeCell ref="AQ2:AS2"/>
+    <mergeCell ref="AC2:AF2"/>
+    <mergeCell ref="D2:J2"/>
+    <mergeCell ref="T2:AA2"/>
+    <mergeCell ref="L2:R2"/>
+    <mergeCell ref="AH2:AO2"/>
+    <mergeCell ref="C3:J10"/>
+    <mergeCell ref="K11:R18"/>
+    <mergeCell ref="S19:AA27"/>
+    <mergeCell ref="T3:AA3"/>
+    <mergeCell ref="BE3:BH3"/>
+    <mergeCell ref="D11:J11"/>
+    <mergeCell ref="D19:J19"/>
+    <mergeCell ref="A29:A32"/>
+    <mergeCell ref="A34:A41"/>
+    <mergeCell ref="A43:A45"/>
+    <mergeCell ref="A47:A51"/>
+    <mergeCell ref="A53:A55"/>
+    <mergeCell ref="A94:A95"/>
+    <mergeCell ref="A57:A60"/>
+    <mergeCell ref="A62:A65"/>
+    <mergeCell ref="A67:A73"/>
+    <mergeCell ref="A75:A77"/>
+    <mergeCell ref="A79:A85"/>
+    <mergeCell ref="A89:A92"/>
+    <mergeCell ref="CP2:CQ2"/>
+    <mergeCell ref="BJ2:BM2"/>
+    <mergeCell ref="CK2:CN2"/>
+    <mergeCell ref="BO2:BU2"/>
+    <mergeCell ref="CA2:CG2"/>
+    <mergeCell ref="BW2:BY2"/>
+    <mergeCell ref="AB28:AF32"/>
+    <mergeCell ref="AG33:AO41"/>
+    <mergeCell ref="AP42:AS45"/>
+    <mergeCell ref="AC3:AF3"/>
+    <mergeCell ref="AH3:AO3"/>
+    <mergeCell ref="AQ3:AS3"/>
+    <mergeCell ref="AU3:AY3"/>
+    <mergeCell ref="BA3:BC3"/>
+    <mergeCell ref="CP3:CQ3"/>
+    <mergeCell ref="CK11:CN11"/>
+    <mergeCell ref="CP11:CQ11"/>
+    <mergeCell ref="BJ11:BM11"/>
+    <mergeCell ref="BO11:BU11"/>
+    <mergeCell ref="BW11:BY11"/>
+    <mergeCell ref="CA11:CG11"/>
+    <mergeCell ref="BJ3:BM3"/>
+    <mergeCell ref="BO3:BU3"/>
+    <mergeCell ref="BW3:BY3"/>
     <mergeCell ref="CH86:CI87"/>
     <mergeCell ref="CJ88:CN92"/>
     <mergeCell ref="CO93:CQ95"/>
@@ -27502,234 +27687,25 @@
     <mergeCell ref="CA93:CG93"/>
     <mergeCell ref="BW93:BY93"/>
     <mergeCell ref="BO88:BU88"/>
-    <mergeCell ref="CP2:CQ2"/>
-    <mergeCell ref="BJ2:BM2"/>
-    <mergeCell ref="CK2:CN2"/>
-    <mergeCell ref="BO2:BU2"/>
-    <mergeCell ref="CA2:CG2"/>
-    <mergeCell ref="BW2:BY2"/>
-    <mergeCell ref="AB28:AF32"/>
-    <mergeCell ref="AG33:AO41"/>
-    <mergeCell ref="AP42:AS45"/>
-    <mergeCell ref="AC3:AF3"/>
-    <mergeCell ref="AH3:AO3"/>
-    <mergeCell ref="AQ3:AS3"/>
-    <mergeCell ref="AU3:AY3"/>
-    <mergeCell ref="BA3:BC3"/>
-    <mergeCell ref="CP3:CQ3"/>
-    <mergeCell ref="CK11:CN11"/>
-    <mergeCell ref="CP11:CQ11"/>
-    <mergeCell ref="BJ11:BM11"/>
-    <mergeCell ref="BO11:BU11"/>
-    <mergeCell ref="BW11:BY11"/>
-    <mergeCell ref="CA11:CG11"/>
-    <mergeCell ref="BJ3:BM3"/>
-    <mergeCell ref="BO3:BU3"/>
-    <mergeCell ref="BW3:BY3"/>
-    <mergeCell ref="A29:A32"/>
-    <mergeCell ref="A34:A41"/>
-    <mergeCell ref="A43:A45"/>
-    <mergeCell ref="A47:A51"/>
-    <mergeCell ref="A53:A55"/>
-    <mergeCell ref="A94:A95"/>
-    <mergeCell ref="A57:A60"/>
-    <mergeCell ref="A62:A65"/>
-    <mergeCell ref="A67:A73"/>
-    <mergeCell ref="A75:A77"/>
-    <mergeCell ref="A79:A85"/>
-    <mergeCell ref="A89:A92"/>
-    <mergeCell ref="A20:A27"/>
-    <mergeCell ref="A12:A18"/>
-    <mergeCell ref="A4:A10"/>
-    <mergeCell ref="BE2:BH2"/>
-    <mergeCell ref="BA2:BC2"/>
-    <mergeCell ref="AU2:AY2"/>
-    <mergeCell ref="AQ2:AS2"/>
-    <mergeCell ref="AC2:AF2"/>
-    <mergeCell ref="D2:J2"/>
-    <mergeCell ref="T2:AA2"/>
-    <mergeCell ref="L2:R2"/>
-    <mergeCell ref="AH2:AO2"/>
-    <mergeCell ref="C3:J10"/>
-    <mergeCell ref="K11:R18"/>
-    <mergeCell ref="S19:AA27"/>
-    <mergeCell ref="T3:AA3"/>
-    <mergeCell ref="BE3:BH3"/>
-    <mergeCell ref="D11:J11"/>
-    <mergeCell ref="D19:J19"/>
-    <mergeCell ref="CA3:CG3"/>
-    <mergeCell ref="CK19:CN19"/>
-    <mergeCell ref="CP19:CQ19"/>
-    <mergeCell ref="BA19:BC19"/>
-    <mergeCell ref="BE19:BH19"/>
-    <mergeCell ref="BJ19:BM19"/>
-    <mergeCell ref="BO19:BU19"/>
-    <mergeCell ref="T11:AA11"/>
-    <mergeCell ref="L3:R3"/>
-    <mergeCell ref="BW19:BY19"/>
-    <mergeCell ref="CA19:CG19"/>
-    <mergeCell ref="L19:R19"/>
-    <mergeCell ref="AC19:AF19"/>
-    <mergeCell ref="AH19:AO19"/>
-    <mergeCell ref="AQ19:AS19"/>
-    <mergeCell ref="AU19:AY19"/>
-    <mergeCell ref="AQ11:AS11"/>
-    <mergeCell ref="AU11:AY11"/>
-    <mergeCell ref="BA11:BC11"/>
-    <mergeCell ref="BE11:BH11"/>
-    <mergeCell ref="AC11:AF11"/>
-    <mergeCell ref="AH11:AO11"/>
-    <mergeCell ref="CK3:CN3"/>
-    <mergeCell ref="BA74:BC74"/>
-    <mergeCell ref="AQ66:AS66"/>
-    <mergeCell ref="AU66:AY66"/>
-    <mergeCell ref="D78:J78"/>
-    <mergeCell ref="L78:R78"/>
-    <mergeCell ref="BW28:BY28"/>
-    <mergeCell ref="CA28:CG28"/>
-    <mergeCell ref="CK28:CN28"/>
-    <mergeCell ref="CP28:CQ28"/>
-    <mergeCell ref="D28:J28"/>
-    <mergeCell ref="T28:AA28"/>
-    <mergeCell ref="L28:R28"/>
-    <mergeCell ref="BA28:BC28"/>
-    <mergeCell ref="AU28:AY28"/>
-    <mergeCell ref="AQ28:AS28"/>
-    <mergeCell ref="AH28:AO28"/>
-    <mergeCell ref="BO28:BU28"/>
-    <mergeCell ref="BJ28:BM28"/>
-    <mergeCell ref="BE28:BH28"/>
-    <mergeCell ref="T56:AA56"/>
-    <mergeCell ref="L56:R56"/>
-    <mergeCell ref="D56:J56"/>
-    <mergeCell ref="BA56:BC56"/>
-    <mergeCell ref="AU56:AY56"/>
-    <mergeCell ref="T66:AA66"/>
-    <mergeCell ref="AC74:AF74"/>
-    <mergeCell ref="T74:AA74"/>
-    <mergeCell ref="L74:R74"/>
-    <mergeCell ref="D74:J74"/>
-    <mergeCell ref="AU74:AY74"/>
-    <mergeCell ref="AQ74:AS74"/>
-    <mergeCell ref="AH74:AO74"/>
-    <mergeCell ref="AH66:AO66"/>
-    <mergeCell ref="BJ88:BM88"/>
-    <mergeCell ref="CA88:CG88"/>
-    <mergeCell ref="BW88:BY88"/>
-    <mergeCell ref="CP88:CQ88"/>
-    <mergeCell ref="AH93:AO93"/>
-    <mergeCell ref="AC93:AF93"/>
-    <mergeCell ref="CK93:CN93"/>
-    <mergeCell ref="BE88:BH88"/>
-    <mergeCell ref="BA88:BC88"/>
-    <mergeCell ref="AU88:AY88"/>
-    <mergeCell ref="AQ88:AS88"/>
-    <mergeCell ref="AH88:AO88"/>
-    <mergeCell ref="AC88:AF88"/>
-    <mergeCell ref="D93:J93"/>
-    <mergeCell ref="BA93:BC93"/>
-    <mergeCell ref="AU93:AY93"/>
-    <mergeCell ref="AQ93:AS93"/>
-    <mergeCell ref="BO93:BU93"/>
-    <mergeCell ref="BJ93:BM93"/>
-    <mergeCell ref="BE93:BH93"/>
-    <mergeCell ref="T93:AA93"/>
-    <mergeCell ref="L93:R93"/>
-    <mergeCell ref="T88:AA88"/>
-    <mergeCell ref="L88:R88"/>
-    <mergeCell ref="D88:J88"/>
-    <mergeCell ref="AU86:AY86"/>
-    <mergeCell ref="AQ86:AS86"/>
-    <mergeCell ref="AH86:AO86"/>
-    <mergeCell ref="AC86:AF86"/>
-    <mergeCell ref="T86:AA86"/>
-    <mergeCell ref="L86:R86"/>
-    <mergeCell ref="D86:J86"/>
-    <mergeCell ref="AQ78:AS78"/>
-    <mergeCell ref="AC52:AF52"/>
-    <mergeCell ref="T52:AA52"/>
-    <mergeCell ref="L52:R52"/>
-    <mergeCell ref="D52:J52"/>
-    <mergeCell ref="AU52:AY52"/>
-    <mergeCell ref="AQ52:AS52"/>
-    <mergeCell ref="AH52:AO52"/>
-    <mergeCell ref="CA52:CG52"/>
-    <mergeCell ref="BW52:BY52"/>
-    <mergeCell ref="BO52:BU52"/>
-    <mergeCell ref="BJ52:BM52"/>
-    <mergeCell ref="BE52:BH52"/>
-    <mergeCell ref="AZ52:BC55"/>
-    <mergeCell ref="AU78:AY78"/>
-    <mergeCell ref="BA78:BC78"/>
-    <mergeCell ref="BE78:BH78"/>
-    <mergeCell ref="BJ78:BM78"/>
-    <mergeCell ref="T78:AA78"/>
-    <mergeCell ref="AC78:AF78"/>
-    <mergeCell ref="AH78:AO78"/>
-    <mergeCell ref="L66:R66"/>
-    <mergeCell ref="D66:J66"/>
-    <mergeCell ref="AC66:AF66"/>
-    <mergeCell ref="D46:J46"/>
-    <mergeCell ref="L46:R46"/>
-    <mergeCell ref="T46:AA46"/>
-    <mergeCell ref="AC46:AF46"/>
-    <mergeCell ref="AH42:AO42"/>
-    <mergeCell ref="AC42:AF42"/>
-    <mergeCell ref="T42:AA42"/>
-    <mergeCell ref="L42:R42"/>
-    <mergeCell ref="D42:J42"/>
-    <mergeCell ref="AU42:AY42"/>
-    <mergeCell ref="BO42:BU42"/>
-    <mergeCell ref="BJ42:BM42"/>
-    <mergeCell ref="CA42:CG42"/>
-    <mergeCell ref="BW42:BY42"/>
-    <mergeCell ref="CP42:CQ42"/>
-    <mergeCell ref="CK42:CN42"/>
-    <mergeCell ref="AH46:AO46"/>
-    <mergeCell ref="AQ46:AS46"/>
-    <mergeCell ref="CA46:CG46"/>
-    <mergeCell ref="CK46:CN46"/>
-    <mergeCell ref="CP46:CQ46"/>
-    <mergeCell ref="BJ46:BM46"/>
-    <mergeCell ref="BO46:BU46"/>
-    <mergeCell ref="BW46:BY46"/>
-    <mergeCell ref="BA46:BC46"/>
-    <mergeCell ref="BE46:BH46"/>
-    <mergeCell ref="AT46:AY51"/>
-    <mergeCell ref="L33:R33"/>
-    <mergeCell ref="D33:J33"/>
-    <mergeCell ref="AC33:AF33"/>
-    <mergeCell ref="T33:AA33"/>
-    <mergeCell ref="BA33:BC33"/>
-    <mergeCell ref="AU33:AY33"/>
-    <mergeCell ref="AQ33:AS33"/>
-    <mergeCell ref="BO33:BU33"/>
-    <mergeCell ref="BJ33:BM33"/>
-    <mergeCell ref="BE33:BH33"/>
-    <mergeCell ref="BO86:BU86"/>
-    <mergeCell ref="BJ86:BM86"/>
-    <mergeCell ref="BE86:BH86"/>
-    <mergeCell ref="BA86:BC86"/>
-    <mergeCell ref="CA86:CG86"/>
-    <mergeCell ref="BW86:BY86"/>
-    <mergeCell ref="CP86:CQ86"/>
-    <mergeCell ref="CK86:CN86"/>
-    <mergeCell ref="CA33:CG33"/>
-    <mergeCell ref="BW33:BY33"/>
-    <mergeCell ref="CP33:CQ33"/>
-    <mergeCell ref="CK33:CN33"/>
-    <mergeCell ref="BE42:BH42"/>
-    <mergeCell ref="BA42:BC42"/>
-    <mergeCell ref="CP52:CQ52"/>
-    <mergeCell ref="CK52:CN52"/>
-    <mergeCell ref="CK66:CN66"/>
-    <mergeCell ref="CP66:CQ66"/>
-    <mergeCell ref="CA66:CG66"/>
-    <mergeCell ref="BJ66:BM66"/>
-    <mergeCell ref="BW66:BY66"/>
-    <mergeCell ref="BA66:BC66"/>
-    <mergeCell ref="BE66:BH66"/>
-    <mergeCell ref="BW78:BY78"/>
+    <mergeCell ref="AQ56:AS56"/>
+    <mergeCell ref="AH56:AO56"/>
+    <mergeCell ref="AC56:AF56"/>
+    <mergeCell ref="CP56:CQ56"/>
+    <mergeCell ref="CK56:CN56"/>
+    <mergeCell ref="CA56:CG56"/>
+    <mergeCell ref="BW56:BY56"/>
+    <mergeCell ref="BO56:BU56"/>
+    <mergeCell ref="BJ56:BM56"/>
+    <mergeCell ref="D61:J61"/>
+    <mergeCell ref="AQ61:AS61"/>
+    <mergeCell ref="AU61:AY61"/>
+    <mergeCell ref="BA61:BC61"/>
+    <mergeCell ref="BE61:BH61"/>
+    <mergeCell ref="BO61:BU61"/>
+    <mergeCell ref="AC61:AF61"/>
+    <mergeCell ref="AH61:AO61"/>
+    <mergeCell ref="L61:R61"/>
+    <mergeCell ref="T61:AA61"/>
   </mergeCells>
   <conditionalFormatting sqref="D93 D94:CN95 D89:CI92 D82:BH82 BJ82:BV82 BA68:BM68 CA65:CQ65 D62:BH65 D79:BV81 D83:BV85 K4:CQ10 D11 D12:J18 S12:CQ18 D19 D20:R27 AB20:CQ27 D28 D29:AA32 D33 D42 AT43:CQ45 D46 D47:AS51 D52 D53:AY55 BD53:CQ55 D56 D57:BC60 BI57:CQ60 D61 BN65:BY65 D66 D67:AG73 BV67:CQ73 D74 D75:BU77 BY75:CQ77 CH79:CQ85 D78 D86 D87:CG87 CJ87:CQ87 D88 CO89:CQ92 CH93:CK93 S11:T11 CO11:CP11 BN11:BO11 BV11:BW11 BZ11:CA11 CH11:CK11 AT11:AU11 AZ11:BA11 BD11:BE11 BI11:BJ11 AG11:AH11 AP11:AQ11 AB11:AC11 K11 AB19:AC19 BZ19:CA19 CH19:CK19 CO19:CP19 BD19:BE19 BI19:BJ19 BN19:BO19 BV19:BW19 K19:L19 S19 AG19:AH19 AP19:AQ19 AT19:AU19 AZ19:BA19 AG28:AH28 BZ28:CA28 CH28:CK28 CO28:CP28 K28:L28 AB28 S28:T28 BD28:BE28 AZ28:BA28 AT28:AU28 AP28:AQ28 BV28:BW28 BN28:BO28 BI28:BJ28 AG32:BC32 BE32:CQ32 AG29:CQ31 AB56:AC56 S56:T56 K56:L56 BD56 AZ56:BA56 AT56:AU56 AP56:AQ56 AG56:AH56 BI56:BJ56 CO56:CP56 CH56:CK56 BZ56:CA56 BV56:BW56 BN56:BO56 BN61:BO61 CH61:CK61 CO61:CP61 BN62:CQ64 BZ61:CA61 AT61:AU61 AZ61:BA61 BD61:BE61 BI61 BV61:BW61 AG61:AH61 AP61:AQ61 S61:T61 AB61:AC61 K61:L61 BY74:CA74 CH74:CK74 AG74:AH74 AB74:AC74 S74:T74 K74:L74 AZ74:BA74 AT74:AU74 AP74:AQ74 BN74:BO74 BI74:BJ74 BD74:BE74 BV74 CO74:CP74 CH78:CK78 CO78:CP78 BV78:BW78 BZ78 AT78:AU78 AZ78:BA78 BD78:BE78 BI78:BJ78 BN78:BO78 AB78:AC78 AG78:AH78 AP78:AQ78 K78:L78 S78:T78 BI88:BJ88 BD88:BE88 AZ88:BA88 AT88:AU88 AP88:AQ88 AG88:AH88 AB88:AC88 S88:T88 K88:L88 BV88:BW88 BN88:BO88 CH88:CJ88 BZ88:CA88 CO88:CP88 AP93:AQ93 AG93:AH93 AB93:AC93 S93:T93 K93:L93 BD93:BE93 AZ93:BA93 AT93:AU93 BV93:BW93 BN93:BO93 BI93:BJ93 BZ93:CA93 CO93 BJ79:BM85 BV66:BW66 CO66:CP66 CH66:CK66 BN66 BZ66:CA66 BD66:BE66 BI66:BJ66 AT66:AU66 AZ66:BA66 AG66:AH66 AP66:AQ66 AB66:AC66 K66:L66 S66:T66 AG52:AH52 AB52:AC52 S52:T52 K52:L52 AZ52 AT52:AU52 AP52:AQ52 BD52:BE52 CH52:CK52 BZ52:CA52 BV52:BW52 BN52:BO52 BI52:BJ52 CO52:CP52 AZ46:BA46 CH46:CK46 CO46:CP46 BN46:BO46 BV46:BW46 BZ46:CA46 BD46:BE46 BI46:BJ46 AP46:AQ46 AT46 K46:L46 S46:T46 AB46:AC46 AG46:AH46 AZ47:CQ51 AP42 AG42:AH42 AB42:AC42 S42:T42 K42:L42 D43:AO43 D44:AF44 AH44:AO44 D45:AO45 AT42:AU42 BI42:BJ42 BD42:BE42 AZ42:BA42 BV42:BW42 BN42:BO42 CH42:CK42 BZ42:CA42 CO42:CP42 S33:T33 K33:L33 AG33 AB33:AC33 AP33:AQ33 BD33:BE33 AZ33:BA33 AT33:AU33 BV33:BW33 BN33:BO33 BI33:BJ33 CH33:CK33 BZ33:CA33 CO33:CP33 AP38:CQ41 AP37:BM37 BO37:CQ37 AP34:CQ36 AZ86:BA86 AT86:AU86 AP86:AQ86 AG86:AH86 AB86:AC86 S86:T86 K86:L86 BV86:BW86 BN86:BO86 BI86:BJ86 BD86:BE86 CH86 BZ86:CA86 CJ86:CK86 CO86:CP86 D34:AF41 AP67:AP73 AT67:AT73 BA67:BC73 AZ67:BM67 AZ69:BM73">
     <cfRule type="cellIs" dxfId="54" priority="72" operator="equal">

</xml_diff>